<commit_message>
Create new branch, don't push to main
Create new branch, don't push to main
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\ts_standard_library\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Jones\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD29644-96F7-4B04-932B-C99C0D4729BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458A251B-F54D-4C35-A52A-1968A6C20333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="1006">
   <si>
     <t>Part Number</t>
   </si>
@@ -3068,6 +3068,9 @@
   </si>
   <si>
     <t>35V</t>
+  </si>
+  <si>
+    <t>Complex IC</t>
   </si>
 </sst>
 </file>
@@ -3449,23 +3452,23 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T185"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -3551,7 +3554,7 @@
       </c>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -3587,7 +3590,7 @@
       </c>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -3623,7 +3626,7 @@
       </c>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
@@ -3659,7 +3662,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -3695,7 +3698,7 @@
       </c>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -3731,7 +3734,7 @@
       </c>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3767,7 +3770,7 @@
       </c>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
@@ -3803,7 +3806,7 @@
       </c>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -3839,7 +3842,7 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -3875,7 +3878,7 @@
       </c>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -3911,7 +3914,7 @@
       </c>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -3947,7 +3950,7 @@
       </c>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -3983,7 +3986,7 @@
       </c>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -4019,7 +4022,7 @@
       </c>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -4055,7 +4058,7 @@
       </c>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>103</v>
       </c>
@@ -4091,7 +4094,7 @@
       </c>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
@@ -4127,7 +4130,7 @@
       </c>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -4163,7 +4166,7 @@
       </c>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -4199,7 +4202,7 @@
       </c>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>115</v>
       </c>
@@ -4235,7 +4238,7 @@
       </c>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
@@ -4271,7 +4274,7 @@
       </c>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -4307,7 +4310,7 @@
       </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>124</v>
       </c>
@@ -4343,7 +4346,7 @@
       </c>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -4379,7 +4382,7 @@
       </c>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
@@ -4415,7 +4418,7 @@
       </c>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>133</v>
       </c>
@@ -4451,7 +4454,7 @@
       </c>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -4487,7 +4490,7 @@
       </c>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
@@ -4523,7 +4526,7 @@
       </c>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>142</v>
       </c>
@@ -4559,7 +4562,7 @@
       </c>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
@@ -4595,7 +4598,7 @@
       </c>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>148</v>
       </c>
@@ -4631,7 +4634,7 @@
       </c>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
@@ -4667,7 +4670,7 @@
       </c>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -4703,7 +4706,7 @@
       </c>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>157</v>
       </c>
@@ -4739,7 +4742,7 @@
       </c>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -4775,7 +4778,7 @@
       </c>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -4811,7 +4814,7 @@
       </c>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>166</v>
       </c>
@@ -4847,7 +4850,7 @@
       </c>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>169</v>
       </c>
@@ -4883,7 +4886,7 @@
       </c>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>172</v>
       </c>
@@ -4919,7 +4922,7 @@
       </c>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>175</v>
       </c>
@@ -4955,7 +4958,7 @@
       </c>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>178</v>
       </c>
@@ -4991,7 +4994,7 @@
       </c>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>181</v>
       </c>
@@ -5027,7 +5030,7 @@
       </c>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>184</v>
       </c>
@@ -5063,7 +5066,7 @@
       </c>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>187</v>
       </c>
@@ -5099,7 +5102,7 @@
       </c>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>190</v>
       </c>
@@ -5135,7 +5138,7 @@
       </c>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>193</v>
       </c>
@@ -5171,7 +5174,7 @@
       </c>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>196</v>
       </c>
@@ -5207,7 +5210,7 @@
       </c>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>199</v>
       </c>
@@ -5243,7 +5246,7 @@
       </c>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>202</v>
       </c>
@@ -5279,7 +5282,7 @@
       </c>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>205</v>
       </c>
@@ -5315,7 +5318,7 @@
       </c>
       <c r="T51" s="1"/>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>208</v>
       </c>
@@ -5351,7 +5354,7 @@
       </c>
       <c r="T52" s="1"/>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>211</v>
       </c>
@@ -5387,7 +5390,7 @@
       </c>
       <c r="T53" s="1"/>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>214</v>
       </c>
@@ -5423,7 +5426,7 @@
       </c>
       <c r="T54" s="1"/>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>217</v>
       </c>
@@ -5459,7 +5462,7 @@
       </c>
       <c r="T55" s="1"/>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>220</v>
       </c>
@@ -5495,7 +5498,7 @@
       </c>
       <c r="T56" s="1"/>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>223</v>
       </c>
@@ -5531,7 +5534,7 @@
       </c>
       <c r="T57" s="1"/>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -5567,7 +5570,7 @@
       </c>
       <c r="T58" s="1"/>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>228</v>
       </c>
@@ -5603,7 +5606,7 @@
       </c>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>231</v>
       </c>
@@ -5639,7 +5642,7 @@
       </c>
       <c r="T60" s="1"/>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
@@ -5675,7 +5678,7 @@
       </c>
       <c r="T61" s="1"/>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>237</v>
       </c>
@@ -5711,7 +5714,7 @@
       </c>
       <c r="T62" s="1"/>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>240</v>
       </c>
@@ -5747,7 +5750,7 @@
       </c>
       <c r="T63" s="1"/>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>243</v>
       </c>
@@ -5783,7 +5786,7 @@
       </c>
       <c r="T64" s="1"/>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>246</v>
       </c>
@@ -5819,7 +5822,7 @@
       </c>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>249</v>
       </c>
@@ -5855,7 +5858,7 @@
       </c>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>252</v>
       </c>
@@ -5891,7 +5894,7 @@
       </c>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>255</v>
       </c>
@@ -5927,7 +5930,7 @@
       </c>
       <c r="T68" s="1"/>
     </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>258</v>
       </c>
@@ -5963,7 +5966,7 @@
       </c>
       <c r="T69" s="1"/>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>261</v>
       </c>
@@ -5999,7 +6002,7 @@
       </c>
       <c r="T70" s="1"/>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>264</v>
       </c>
@@ -6035,7 +6038,7 @@
       </c>
       <c r="T71" s="1"/>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>267</v>
       </c>
@@ -6071,7 +6074,7 @@
       </c>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>270</v>
       </c>
@@ -6107,7 +6110,7 @@
       </c>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>273</v>
       </c>
@@ -6143,7 +6146,7 @@
       </c>
       <c r="T74" s="1"/>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>276</v>
       </c>
@@ -6179,7 +6182,7 @@
       </c>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>279</v>
       </c>
@@ -6215,7 +6218,7 @@
       </c>
       <c r="T76" s="1"/>
     </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6251,7 +6254,7 @@
       </c>
       <c r="T77" s="1"/>
     </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6287,7 +6290,7 @@
       </c>
       <c r="T78" s="1"/>
     </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>288</v>
       </c>
@@ -6323,7 +6326,7 @@
       </c>
       <c r="T79" s="1"/>
     </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>291</v>
       </c>
@@ -6359,7 +6362,7 @@
       </c>
       <c r="T80" s="1"/>
     </row>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>294</v>
       </c>
@@ -6395,7 +6398,7 @@
       </c>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>297</v>
       </c>
@@ -6431,7 +6434,7 @@
       </c>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>300</v>
       </c>
@@ -6467,7 +6470,7 @@
       </c>
       <c r="T83" s="1"/>
     </row>
-    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>303</v>
       </c>
@@ -6503,7 +6506,7 @@
       </c>
       <c r="T84" s="1"/>
     </row>
-    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>306</v>
       </c>
@@ -6539,7 +6542,7 @@
       </c>
       <c r="T85" s="1"/>
     </row>
-    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>309</v>
       </c>
@@ -6575,7 +6578,7 @@
       </c>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>312</v>
       </c>
@@ -6611,7 +6614,7 @@
       </c>
       <c r="T87" s="1"/>
     </row>
-    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>315</v>
       </c>
@@ -6647,7 +6650,7 @@
       </c>
       <c r="T88" s="1"/>
     </row>
-    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>318</v>
       </c>
@@ -6683,7 +6686,7 @@
       </c>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>321</v>
       </c>
@@ -6719,7 +6722,7 @@
       </c>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>324</v>
       </c>
@@ -6755,7 +6758,7 @@
       </c>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>327</v>
       </c>
@@ -6791,7 +6794,7 @@
       </c>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>330</v>
       </c>
@@ -6827,7 +6830,7 @@
       </c>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>333</v>
       </c>
@@ -6863,7 +6866,7 @@
       </c>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>336</v>
       </c>
@@ -6899,7 +6902,7 @@
       </c>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>339</v>
       </c>
@@ -6935,7 +6938,7 @@
       </c>
       <c r="T96" s="1"/>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>342</v>
       </c>
@@ -6971,7 +6974,7 @@
       </c>
       <c r="T97" s="1"/>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>345</v>
       </c>
@@ -7007,7 +7010,7 @@
       </c>
       <c r="T98" s="1"/>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>348</v>
       </c>
@@ -7043,7 +7046,7 @@
       </c>
       <c r="T99" s="1"/>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>351</v>
       </c>
@@ -7079,7 +7082,7 @@
       </c>
       <c r="T100" s="1"/>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>354</v>
       </c>
@@ -7115,7 +7118,7 @@
       </c>
       <c r="T101" s="1"/>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>357</v>
       </c>
@@ -7151,7 +7154,7 @@
       </c>
       <c r="T102" s="1"/>
     </row>
-    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>360</v>
       </c>
@@ -7187,7 +7190,7 @@
       </c>
       <c r="T103" s="1"/>
     </row>
-    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>363</v>
       </c>
@@ -7223,7 +7226,7 @@
       </c>
       <c r="T104" s="1"/>
     </row>
-    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>366</v>
       </c>
@@ -7259,7 +7262,7 @@
       </c>
       <c r="T105" s="1"/>
     </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>369</v>
       </c>
@@ -7295,7 +7298,7 @@
       </c>
       <c r="T106" s="1"/>
     </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>372</v>
       </c>
@@ -7331,7 +7334,7 @@
       </c>
       <c r="T107" s="1"/>
     </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>375</v>
       </c>
@@ -7367,7 +7370,7 @@
       </c>
       <c r="T108" s="1"/>
     </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>378</v>
       </c>
@@ -7403,7 +7406,7 @@
       </c>
       <c r="T109" s="1"/>
     </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>381</v>
       </c>
@@ -7439,7 +7442,7 @@
       </c>
       <c r="T110" s="1"/>
     </row>
-    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>384</v>
       </c>
@@ -7475,7 +7478,7 @@
       </c>
       <c r="T111" s="1"/>
     </row>
-    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>387</v>
       </c>
@@ -7511,7 +7514,7 @@
       </c>
       <c r="T112" s="1"/>
     </row>
-    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>390</v>
       </c>
@@ -7547,7 +7550,7 @@
       </c>
       <c r="T113" s="1"/>
     </row>
-    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>393</v>
       </c>
@@ -7583,7 +7586,7 @@
       </c>
       <c r="T114" s="1"/>
     </row>
-    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>396</v>
       </c>
@@ -7619,7 +7622,7 @@
       </c>
       <c r="T115" s="1"/>
     </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>399</v>
       </c>
@@ -7655,7 +7658,7 @@
       </c>
       <c r="T116" s="1"/>
     </row>
-    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>402</v>
       </c>
@@ -7691,7 +7694,7 @@
       </c>
       <c r="T117" s="1"/>
     </row>
-    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>402</v>
       </c>
@@ -7727,7 +7730,7 @@
       </c>
       <c r="T118" s="1"/>
     </row>
-    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>407</v>
       </c>
@@ -7763,7 +7766,7 @@
       </c>
       <c r="T119" s="1"/>
     </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>410</v>
       </c>
@@ -7799,7 +7802,7 @@
       </c>
       <c r="T120" s="1"/>
     </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>413</v>
       </c>
@@ -7835,7 +7838,7 @@
       </c>
       <c r="T121" s="1"/>
     </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>416</v>
       </c>
@@ -7872,7 +7875,7 @@
       </c>
       <c r="T122" s="1"/>
     </row>
-    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>419</v>
       </c>
@@ -7909,7 +7912,7 @@
       </c>
       <c r="T123" s="1"/>
     </row>
-    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>422</v>
       </c>
@@ -7946,7 +7949,7 @@
       </c>
       <c r="T124" s="1"/>
     </row>
-    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>424</v>
       </c>
@@ -7983,7 +7986,7 @@
       </c>
       <c r="T125" s="1"/>
     </row>
-    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>427</v>
       </c>
@@ -8020,7 +8023,7 @@
       </c>
       <c r="T126" s="1"/>
     </row>
-    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>430</v>
       </c>
@@ -8057,7 +8060,7 @@
       </c>
       <c r="T127" s="1"/>
     </row>
-    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>433</v>
       </c>
@@ -8094,7 +8097,7 @@
       </c>
       <c r="T128" s="1"/>
     </row>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>436</v>
       </c>
@@ -8131,7 +8134,7 @@
       </c>
       <c r="T129" s="1"/>
     </row>
-    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>439</v>
       </c>
@@ -8168,7 +8171,7 @@
       </c>
       <c r="T130" s="1"/>
     </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>442</v>
       </c>
@@ -8205,7 +8208,7 @@
       </c>
       <c r="T131" s="1"/>
     </row>
-    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>445</v>
       </c>
@@ -8242,7 +8245,7 @@
       </c>
       <c r="T132" s="1"/>
     </row>
-    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>448</v>
       </c>
@@ -8279,7 +8282,7 @@
       </c>
       <c r="T133" s="1"/>
     </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>451</v>
       </c>
@@ -8316,7 +8319,7 @@
       </c>
       <c r="T134" s="1"/>
     </row>
-    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>454</v>
       </c>
@@ -8353,7 +8356,7 @@
       </c>
       <c r="T135" s="1"/>
     </row>
-    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>457</v>
       </c>
@@ -8390,7 +8393,7 @@
       </c>
       <c r="T136" s="1"/>
     </row>
-    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>460</v>
       </c>
@@ -8427,7 +8430,7 @@
       </c>
       <c r="T137" s="1"/>
     </row>
-    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>463</v>
       </c>
@@ -8464,7 +8467,7 @@
       </c>
       <c r="T138" s="1"/>
     </row>
-    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>466</v>
       </c>
@@ -8501,7 +8504,7 @@
       </c>
       <c r="T139" s="1"/>
     </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>469</v>
       </c>
@@ -8538,7 +8541,7 @@
       </c>
       <c r="T140" s="1"/>
     </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>472</v>
       </c>
@@ -8575,7 +8578,7 @@
       </c>
       <c r="T141" s="1"/>
     </row>
-    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>475</v>
       </c>
@@ -8612,7 +8615,7 @@
       </c>
       <c r="T142" s="1"/>
     </row>
-    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>478</v>
       </c>
@@ -8649,7 +8652,7 @@
       </c>
       <c r="T143" s="1"/>
     </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>481</v>
       </c>
@@ -8686,7 +8689,7 @@
       </c>
       <c r="T144" s="1"/>
     </row>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>484</v>
       </c>
@@ -8723,7 +8726,7 @@
       </c>
       <c r="T145" s="1"/>
     </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>487</v>
       </c>
@@ -8759,7 +8762,7 @@
       </c>
       <c r="T146" s="1"/>
     </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>490</v>
       </c>
@@ -8795,7 +8798,7 @@
       </c>
       <c r="T147" s="1"/>
     </row>
-    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>493</v>
       </c>
@@ -8831,7 +8834,7 @@
       </c>
       <c r="T148" s="1"/>
     </row>
-    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>496</v>
       </c>
@@ -8867,7 +8870,7 @@
       </c>
       <c r="T149" s="1"/>
     </row>
-    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>499</v>
       </c>
@@ -8903,7 +8906,7 @@
       </c>
       <c r="T150" s="1"/>
     </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>502</v>
       </c>
@@ -8939,7 +8942,7 @@
       </c>
       <c r="T151" s="1"/>
     </row>
-    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>505</v>
       </c>
@@ -8975,7 +8978,7 @@
       </c>
       <c r="T152" s="1"/>
     </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>508</v>
       </c>
@@ -9011,7 +9014,7 @@
       </c>
       <c r="T153" s="1"/>
     </row>
-    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>511</v>
       </c>
@@ -9047,7 +9050,7 @@
       </c>
       <c r="T154" s="1"/>
     </row>
-    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>514</v>
       </c>
@@ -9083,7 +9086,7 @@
       </c>
       <c r="T155" s="1"/>
     </row>
-    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>517</v>
       </c>
@@ -9119,7 +9122,7 @@
       </c>
       <c r="T156" s="1"/>
     </row>
-    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>520</v>
       </c>
@@ -9155,7 +9158,7 @@
       </c>
       <c r="T157" s="1"/>
     </row>
-    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>523</v>
       </c>
@@ -9191,7 +9194,7 @@
       </c>
       <c r="T158" s="1"/>
     </row>
-    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>526</v>
       </c>
@@ -9227,7 +9230,7 @@
       </c>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>529</v>
       </c>
@@ -9263,7 +9266,7 @@
       </c>
       <c r="T160" s="1"/>
     </row>
-    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>532</v>
       </c>
@@ -9299,7 +9302,7 @@
       </c>
       <c r="T161" s="1"/>
     </row>
-    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>535</v>
       </c>
@@ -9335,7 +9338,7 @@
       </c>
       <c r="T162" s="1"/>
     </row>
-    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>538</v>
       </c>
@@ -9371,7 +9374,7 @@
       </c>
       <c r="T163" s="1"/>
     </row>
-    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>541</v>
       </c>
@@ -9407,7 +9410,7 @@
       </c>
       <c r="T164" s="1"/>
     </row>
-    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>544</v>
       </c>
@@ -9443,7 +9446,7 @@
       </c>
       <c r="T165" s="1"/>
     </row>
-    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>547</v>
       </c>
@@ -9479,7 +9482,7 @@
       </c>
       <c r="T166" s="1"/>
     </row>
-    <row r="167" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>550</v>
       </c>
@@ -9515,7 +9518,7 @@
       </c>
       <c r="T167" s="1"/>
     </row>
-    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>553</v>
       </c>
@@ -9551,7 +9554,7 @@
       </c>
       <c r="T168" s="1"/>
     </row>
-    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>556</v>
       </c>
@@ -9587,7 +9590,7 @@
       </c>
       <c r="T169" s="1"/>
     </row>
-    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>559</v>
       </c>
@@ -9623,7 +9626,7 @@
       </c>
       <c r="T170" s="1"/>
     </row>
-    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>678</v>
       </c>
@@ -9655,7 +9658,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>733</v>
       </c>
@@ -9690,7 +9693,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>723</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>735</v>
       </c>
@@ -9760,7 +9763,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>730</v>
       </c>
@@ -9795,7 +9798,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>853</v>
       </c>
@@ -9827,7 +9830,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>875</v>
       </c>
@@ -9862,7 +9865,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>940</v>
       </c>
@@ -9897,7 +9900,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>944</v>
       </c>
@@ -9932,7 +9935,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>947</v>
       </c>
@@ -9967,7 +9970,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>953</v>
       </c>
@@ -9999,7 +10002,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>954</v>
       </c>
@@ -10031,7 +10034,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>967</v>
       </c>
@@ -10066,7 +10069,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>980</v>
       </c>
@@ -10101,7 +10104,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>982</v>
       </c>
@@ -10152,660 +10155,730 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="98.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="148" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="98.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="148" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>588</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>582</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>685</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>686</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>685</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>570</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>685</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>579</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>687</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>689</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>690</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>691</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>690</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>570</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>692</v>
       </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
       <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>693</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>695</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>696</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>697</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>696</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>570</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>698</v>
       </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
       <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
         <v>699</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>776</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>775</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>777</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>778</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>570</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>779</v>
       </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
       <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
         <v>781</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>782</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>582</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>783</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>782</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>570</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>784</v>
       </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
       <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
         <v>785</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>582</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>787</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>788</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>787</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>570</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>789</v>
       </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
       <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
         <v>790</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>776</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>818</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>817</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>814</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>570</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>813</v>
       </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
       <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
         <v>816</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>738</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
         <v>819</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>820</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>819</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>570</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>821</v>
       </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
       <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
         <v>822</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>776</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>824</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>828</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>824</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>570</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>825</v>
       </c>
-      <c r="G10" t="s">
-        <v>35</v>
-      </c>
       <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
         <v>826</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>738</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
         <v>845</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>846</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>858</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>570</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>857</v>
       </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
       <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
         <v>847</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>563</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>849</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>850</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>849</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>570</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>873</v>
       </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
       <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
         <v>849</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>935</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>931</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>934</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>931</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>570</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>933</v>
       </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
       <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
         <v>931</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>563</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
         <v>871</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>872</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>871</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>570</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>870</v>
       </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>563</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>949</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>950</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>949</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>570</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>951</v>
       </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
       <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>689</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>962</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>966</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>962</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>570</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>963</v>
       </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
       <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
         <v>965</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>689</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
         <v>974</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>975</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>974</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>570</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>963</v>
       </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>563</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>976</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>978</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>976</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>570</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>979</v>
       </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
       <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>563</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>986</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>987</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>986</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>570</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>990</v>
       </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
       <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
         <v>988</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>738</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
         <v>991</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>820</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>991</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>570</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>821</v>
       </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>689</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>992</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>993</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>992</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>570</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>873</v>
       </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>689</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
         <v>994</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>995</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>996</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>570</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>994</v>
       </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>689</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
         <v>998</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>999</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>998</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>570</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>821</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{815BD2A1-6E8A-46F8-9861-C78A08FF1096}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{EA6EFD7C-549A-44E5-A801-1C9B5F327F6B}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{1F450374-E59F-43AA-8572-ED9007CAF744}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{5F85956A-FEB2-4AD6-B47C-9537FE62885B}"/>
-    <hyperlink ref="I7" r:id="rId5" xr:uid="{71439ED1-BAD7-46B8-9FA2-B26BCC099889}"/>
-    <hyperlink ref="I9" r:id="rId6" xr:uid="{CD33C165-116A-4895-BF42-9E15D8C3F899}"/>
-    <hyperlink ref="I16" r:id="rId7" xr:uid="{E0AFB124-543E-4E34-8464-CF1CC76A6806}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{815BD2A1-6E8A-46F8-9861-C78A08FF1096}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{EA6EFD7C-549A-44E5-A801-1C9B5F327F6B}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{1F450374-E59F-43AA-8572-ED9007CAF744}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{5F85956A-FEB2-4AD6-B47C-9537FE62885B}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{71439ED1-BAD7-46B8-9FA2-B26BCC099889}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{CD33C165-116A-4895-BF42-9E15D8C3F899}"/>
+    <hyperlink ref="J16" r:id="rId7" xr:uid="{E0AFB124-543E-4E34-8464-CF1CC76A6806}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -10820,18 +10893,18 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10878,7 +10951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>672</v>
       </c>
@@ -10923,22 +10996,22 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10988,7 +11061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>562</v>
       </c>
@@ -11023,7 +11096,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>572</v>
       </c>
@@ -11058,7 +11131,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>659</v>
       </c>
@@ -11093,7 +11166,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>737</v>
       </c>
@@ -11128,7 +11201,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>742</v>
       </c>
@@ -11163,7 +11236,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>837</v>
       </c>
@@ -11196,7 +11269,7 @@
       </c>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>881</v>
       </c>
@@ -11245,9 +11318,9 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11316,523 +11389,523 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="21.453125" customWidth="1"/>
-    <col min="258" max="258" width="14.81640625" customWidth="1"/>
-    <col min="259" max="259" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="21.44140625" customWidth="1"/>
+    <col min="258" max="258" width="14.77734375" customWidth="1"/>
+    <col min="259" max="259" width="20.5546875" customWidth="1"/>
     <col min="260" max="260" width="17" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="21.453125" customWidth="1"/>
-    <col min="514" max="514" width="14.81640625" customWidth="1"/>
-    <col min="515" max="515" width="20.54296875" customWidth="1"/>
+    <col min="261" max="261" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="21.44140625" customWidth="1"/>
+    <col min="514" max="514" width="14.77734375" customWidth="1"/>
+    <col min="515" max="515" width="20.5546875" customWidth="1"/>
     <col min="516" max="516" width="17" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="21.453125" customWidth="1"/>
-    <col min="770" max="770" width="14.81640625" customWidth="1"/>
-    <col min="771" max="771" width="20.54296875" customWidth="1"/>
+    <col min="517" max="517" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="21.44140625" customWidth="1"/>
+    <col min="770" max="770" width="14.77734375" customWidth="1"/>
+    <col min="771" max="771" width="20.5546875" customWidth="1"/>
     <col min="772" max="772" width="17" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="775" max="775" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="21.453125" customWidth="1"/>
-    <col min="1026" max="1026" width="14.81640625" customWidth="1"/>
-    <col min="1027" max="1027" width="20.54296875" customWidth="1"/>
+    <col min="773" max="773" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="21.44140625" customWidth="1"/>
+    <col min="1026" max="1026" width="14.77734375" customWidth="1"/>
+    <col min="1027" max="1027" width="20.5546875" customWidth="1"/>
     <col min="1028" max="1028" width="17" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1031" max="1031" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="21.453125" customWidth="1"/>
-    <col min="1282" max="1282" width="14.81640625" customWidth="1"/>
-    <col min="1283" max="1283" width="20.54296875" customWidth="1"/>
+    <col min="1029" max="1029" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="21.44140625" customWidth="1"/>
+    <col min="1282" max="1282" width="14.77734375" customWidth="1"/>
+    <col min="1283" max="1283" width="20.5546875" customWidth="1"/>
     <col min="1284" max="1284" width="17" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1287" max="1287" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="21.453125" customWidth="1"/>
-    <col min="1538" max="1538" width="14.81640625" customWidth="1"/>
-    <col min="1539" max="1539" width="20.54296875" customWidth="1"/>
+    <col min="1285" max="1285" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="21.44140625" customWidth="1"/>
+    <col min="1538" max="1538" width="14.77734375" customWidth="1"/>
+    <col min="1539" max="1539" width="20.5546875" customWidth="1"/>
     <col min="1540" max="1540" width="17" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1543" max="1543" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="21.453125" customWidth="1"/>
-    <col min="1794" max="1794" width="14.81640625" customWidth="1"/>
-    <col min="1795" max="1795" width="20.54296875" customWidth="1"/>
+    <col min="1541" max="1541" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="21.44140625" customWidth="1"/>
+    <col min="1794" max="1794" width="14.77734375" customWidth="1"/>
+    <col min="1795" max="1795" width="20.5546875" customWidth="1"/>
     <col min="1796" max="1796" width="17" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1799" max="1799" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="21.453125" customWidth="1"/>
-    <col min="2050" max="2050" width="14.81640625" customWidth="1"/>
-    <col min="2051" max="2051" width="20.54296875" customWidth="1"/>
+    <col min="1797" max="1797" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="21.44140625" customWidth="1"/>
+    <col min="2050" max="2050" width="14.77734375" customWidth="1"/>
+    <col min="2051" max="2051" width="20.5546875" customWidth="1"/>
     <col min="2052" max="2052" width="17" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2055" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="21.453125" customWidth="1"/>
-    <col min="2306" max="2306" width="14.81640625" customWidth="1"/>
-    <col min="2307" max="2307" width="20.54296875" customWidth="1"/>
+    <col min="2053" max="2053" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="21.44140625" customWidth="1"/>
+    <col min="2306" max="2306" width="14.77734375" customWidth="1"/>
+    <col min="2307" max="2307" width="20.5546875" customWidth="1"/>
     <col min="2308" max="2308" width="17" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2311" max="2311" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="21.453125" customWidth="1"/>
-    <col min="2562" max="2562" width="14.81640625" customWidth="1"/>
-    <col min="2563" max="2563" width="20.54296875" customWidth="1"/>
+    <col min="2309" max="2309" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="21.44140625" customWidth="1"/>
+    <col min="2562" max="2562" width="14.77734375" customWidth="1"/>
+    <col min="2563" max="2563" width="20.5546875" customWidth="1"/>
     <col min="2564" max="2564" width="17" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2567" max="2567" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="21.453125" customWidth="1"/>
-    <col min="2818" max="2818" width="14.81640625" customWidth="1"/>
-    <col min="2819" max="2819" width="20.54296875" customWidth="1"/>
+    <col min="2565" max="2565" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="21.44140625" customWidth="1"/>
+    <col min="2818" max="2818" width="14.77734375" customWidth="1"/>
+    <col min="2819" max="2819" width="20.5546875" customWidth="1"/>
     <col min="2820" max="2820" width="17" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2823" max="2823" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="21.453125" customWidth="1"/>
-    <col min="3074" max="3074" width="14.81640625" customWidth="1"/>
-    <col min="3075" max="3075" width="20.54296875" customWidth="1"/>
+    <col min="2821" max="2821" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="21.44140625" customWidth="1"/>
+    <col min="3074" max="3074" width="14.77734375" customWidth="1"/>
+    <col min="3075" max="3075" width="20.5546875" customWidth="1"/>
     <col min="3076" max="3076" width="17" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3079" max="3079" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="21.453125" customWidth="1"/>
-    <col min="3330" max="3330" width="14.81640625" customWidth="1"/>
-    <col min="3331" max="3331" width="20.54296875" customWidth="1"/>
+    <col min="3077" max="3077" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="21.44140625" customWidth="1"/>
+    <col min="3330" max="3330" width="14.77734375" customWidth="1"/>
+    <col min="3331" max="3331" width="20.5546875" customWidth="1"/>
     <col min="3332" max="3332" width="17" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3335" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="21.453125" customWidth="1"/>
-    <col min="3586" max="3586" width="14.81640625" customWidth="1"/>
-    <col min="3587" max="3587" width="20.54296875" customWidth="1"/>
+    <col min="3333" max="3333" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="21.44140625" customWidth="1"/>
+    <col min="3586" max="3586" width="14.77734375" customWidth="1"/>
+    <col min="3587" max="3587" width="20.5546875" customWidth="1"/>
     <col min="3588" max="3588" width="17" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3591" max="3591" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="21.453125" customWidth="1"/>
-    <col min="3842" max="3842" width="14.81640625" customWidth="1"/>
-    <col min="3843" max="3843" width="20.54296875" customWidth="1"/>
+    <col min="3589" max="3589" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="21.44140625" customWidth="1"/>
+    <col min="3842" max="3842" width="14.77734375" customWidth="1"/>
+    <col min="3843" max="3843" width="20.5546875" customWidth="1"/>
     <col min="3844" max="3844" width="17" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3847" max="3847" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="21.453125" customWidth="1"/>
-    <col min="4098" max="4098" width="14.81640625" customWidth="1"/>
-    <col min="4099" max="4099" width="20.54296875" customWidth="1"/>
+    <col min="3845" max="3845" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="21.44140625" customWidth="1"/>
+    <col min="4098" max="4098" width="14.77734375" customWidth="1"/>
+    <col min="4099" max="4099" width="20.5546875" customWidth="1"/>
     <col min="4100" max="4100" width="17" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4103" max="4103" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="21.453125" customWidth="1"/>
-    <col min="4354" max="4354" width="14.81640625" customWidth="1"/>
-    <col min="4355" max="4355" width="20.54296875" customWidth="1"/>
+    <col min="4101" max="4101" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="21.44140625" customWidth="1"/>
+    <col min="4354" max="4354" width="14.77734375" customWidth="1"/>
+    <col min="4355" max="4355" width="20.5546875" customWidth="1"/>
     <col min="4356" max="4356" width="17" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4359" max="4359" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="21.453125" customWidth="1"/>
-    <col min="4610" max="4610" width="14.81640625" customWidth="1"/>
-    <col min="4611" max="4611" width="20.54296875" customWidth="1"/>
+    <col min="4357" max="4357" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="21.44140625" customWidth="1"/>
+    <col min="4610" max="4610" width="14.77734375" customWidth="1"/>
+    <col min="4611" max="4611" width="20.5546875" customWidth="1"/>
     <col min="4612" max="4612" width="17" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4615" max="4615" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="21.453125" customWidth="1"/>
-    <col min="4866" max="4866" width="14.81640625" customWidth="1"/>
-    <col min="4867" max="4867" width="20.54296875" customWidth="1"/>
+    <col min="4613" max="4613" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="21.44140625" customWidth="1"/>
+    <col min="4866" max="4866" width="14.77734375" customWidth="1"/>
+    <col min="4867" max="4867" width="20.5546875" customWidth="1"/>
     <col min="4868" max="4868" width="17" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4871" max="4871" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="21.453125" customWidth="1"/>
-    <col min="5122" max="5122" width="14.81640625" customWidth="1"/>
-    <col min="5123" max="5123" width="20.54296875" customWidth="1"/>
+    <col min="4869" max="4869" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="21.44140625" customWidth="1"/>
+    <col min="5122" max="5122" width="14.77734375" customWidth="1"/>
+    <col min="5123" max="5123" width="20.5546875" customWidth="1"/>
     <col min="5124" max="5124" width="17" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5127" max="5127" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="21.453125" customWidth="1"/>
-    <col min="5378" max="5378" width="14.81640625" customWidth="1"/>
-    <col min="5379" max="5379" width="20.54296875" customWidth="1"/>
+    <col min="5125" max="5125" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="21.44140625" customWidth="1"/>
+    <col min="5378" max="5378" width="14.77734375" customWidth="1"/>
+    <col min="5379" max="5379" width="20.5546875" customWidth="1"/>
     <col min="5380" max="5380" width="17" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5383" max="5383" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="21.453125" customWidth="1"/>
-    <col min="5634" max="5634" width="14.81640625" customWidth="1"/>
-    <col min="5635" max="5635" width="20.54296875" customWidth="1"/>
+    <col min="5381" max="5381" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="21.44140625" customWidth="1"/>
+    <col min="5634" max="5634" width="14.77734375" customWidth="1"/>
+    <col min="5635" max="5635" width="20.5546875" customWidth="1"/>
     <col min="5636" max="5636" width="17" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5639" max="5639" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="21.453125" customWidth="1"/>
-    <col min="5890" max="5890" width="14.81640625" customWidth="1"/>
-    <col min="5891" max="5891" width="20.54296875" customWidth="1"/>
+    <col min="5637" max="5637" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="21.44140625" customWidth="1"/>
+    <col min="5890" max="5890" width="14.77734375" customWidth="1"/>
+    <col min="5891" max="5891" width="20.5546875" customWidth="1"/>
     <col min="5892" max="5892" width="17" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5895" max="5895" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="21.453125" customWidth="1"/>
-    <col min="6146" max="6146" width="14.81640625" customWidth="1"/>
-    <col min="6147" max="6147" width="20.54296875" customWidth="1"/>
+    <col min="5893" max="5893" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="21.44140625" customWidth="1"/>
+    <col min="6146" max="6146" width="14.77734375" customWidth="1"/>
+    <col min="6147" max="6147" width="20.5546875" customWidth="1"/>
     <col min="6148" max="6148" width="17" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6151" max="6151" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="21.453125" customWidth="1"/>
-    <col min="6402" max="6402" width="14.81640625" customWidth="1"/>
-    <col min="6403" max="6403" width="20.54296875" customWidth="1"/>
+    <col min="6149" max="6149" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="21.44140625" customWidth="1"/>
+    <col min="6402" max="6402" width="14.77734375" customWidth="1"/>
+    <col min="6403" max="6403" width="20.5546875" customWidth="1"/>
     <col min="6404" max="6404" width="17" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6407" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="21.453125" customWidth="1"/>
-    <col min="6658" max="6658" width="14.81640625" customWidth="1"/>
-    <col min="6659" max="6659" width="20.54296875" customWidth="1"/>
+    <col min="6405" max="6405" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="21.44140625" customWidth="1"/>
+    <col min="6658" max="6658" width="14.77734375" customWidth="1"/>
+    <col min="6659" max="6659" width="20.5546875" customWidth="1"/>
     <col min="6660" max="6660" width="17" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6663" max="6663" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="21.453125" customWidth="1"/>
-    <col min="6914" max="6914" width="14.81640625" customWidth="1"/>
-    <col min="6915" max="6915" width="20.54296875" customWidth="1"/>
+    <col min="6661" max="6661" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="21.44140625" customWidth="1"/>
+    <col min="6914" max="6914" width="14.77734375" customWidth="1"/>
+    <col min="6915" max="6915" width="20.5546875" customWidth="1"/>
     <col min="6916" max="6916" width="17" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6919" max="6919" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="21.453125" customWidth="1"/>
-    <col min="7170" max="7170" width="14.81640625" customWidth="1"/>
-    <col min="7171" max="7171" width="20.54296875" customWidth="1"/>
+    <col min="6917" max="6917" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="21.44140625" customWidth="1"/>
+    <col min="7170" max="7170" width="14.77734375" customWidth="1"/>
+    <col min="7171" max="7171" width="20.5546875" customWidth="1"/>
     <col min="7172" max="7172" width="17" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7175" max="7175" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="21.453125" customWidth="1"/>
-    <col min="7426" max="7426" width="14.81640625" customWidth="1"/>
-    <col min="7427" max="7427" width="20.54296875" customWidth="1"/>
+    <col min="7173" max="7173" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="21.44140625" customWidth="1"/>
+    <col min="7426" max="7426" width="14.77734375" customWidth="1"/>
+    <col min="7427" max="7427" width="20.5546875" customWidth="1"/>
     <col min="7428" max="7428" width="17" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7431" max="7431" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="21.453125" customWidth="1"/>
-    <col min="7682" max="7682" width="14.81640625" customWidth="1"/>
-    <col min="7683" max="7683" width="20.54296875" customWidth="1"/>
+    <col min="7429" max="7429" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="21.44140625" customWidth="1"/>
+    <col min="7682" max="7682" width="14.77734375" customWidth="1"/>
+    <col min="7683" max="7683" width="20.5546875" customWidth="1"/>
     <col min="7684" max="7684" width="17" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7687" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="21.453125" customWidth="1"/>
-    <col min="7938" max="7938" width="14.81640625" customWidth="1"/>
-    <col min="7939" max="7939" width="20.54296875" customWidth="1"/>
+    <col min="7685" max="7685" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="21.44140625" customWidth="1"/>
+    <col min="7938" max="7938" width="14.77734375" customWidth="1"/>
+    <col min="7939" max="7939" width="20.5546875" customWidth="1"/>
     <col min="7940" max="7940" width="17" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7943" max="7943" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="21.453125" customWidth="1"/>
-    <col min="8194" max="8194" width="14.81640625" customWidth="1"/>
-    <col min="8195" max="8195" width="20.54296875" customWidth="1"/>
+    <col min="7941" max="7941" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="21.44140625" customWidth="1"/>
+    <col min="8194" max="8194" width="14.77734375" customWidth="1"/>
+    <col min="8195" max="8195" width="20.5546875" customWidth="1"/>
     <col min="8196" max="8196" width="17" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8199" max="8199" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="21.453125" customWidth="1"/>
-    <col min="8450" max="8450" width="14.81640625" customWidth="1"/>
-    <col min="8451" max="8451" width="20.54296875" customWidth="1"/>
+    <col min="8197" max="8197" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="21.44140625" customWidth="1"/>
+    <col min="8450" max="8450" width="14.77734375" customWidth="1"/>
+    <col min="8451" max="8451" width="20.5546875" customWidth="1"/>
     <col min="8452" max="8452" width="17" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8455" max="8455" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="21.453125" customWidth="1"/>
-    <col min="8706" max="8706" width="14.81640625" customWidth="1"/>
-    <col min="8707" max="8707" width="20.54296875" customWidth="1"/>
+    <col min="8453" max="8453" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="21.44140625" customWidth="1"/>
+    <col min="8706" max="8706" width="14.77734375" customWidth="1"/>
+    <col min="8707" max="8707" width="20.5546875" customWidth="1"/>
     <col min="8708" max="8708" width="17" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8711" max="8711" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="21.453125" customWidth="1"/>
-    <col min="8962" max="8962" width="14.81640625" customWidth="1"/>
-    <col min="8963" max="8963" width="20.54296875" customWidth="1"/>
+    <col min="8709" max="8709" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="21.44140625" customWidth="1"/>
+    <col min="8962" max="8962" width="14.77734375" customWidth="1"/>
+    <col min="8963" max="8963" width="20.5546875" customWidth="1"/>
     <col min="8964" max="8964" width="17" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8967" max="8967" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="21.453125" customWidth="1"/>
-    <col min="9218" max="9218" width="14.81640625" customWidth="1"/>
-    <col min="9219" max="9219" width="20.54296875" customWidth="1"/>
+    <col min="8965" max="8965" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="21.44140625" customWidth="1"/>
+    <col min="9218" max="9218" width="14.77734375" customWidth="1"/>
+    <col min="9219" max="9219" width="20.5546875" customWidth="1"/>
     <col min="9220" max="9220" width="17" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9223" max="9223" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="21.453125" customWidth="1"/>
-    <col min="9474" max="9474" width="14.81640625" customWidth="1"/>
-    <col min="9475" max="9475" width="20.54296875" customWidth="1"/>
+    <col min="9221" max="9221" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="21.44140625" customWidth="1"/>
+    <col min="9474" max="9474" width="14.77734375" customWidth="1"/>
+    <col min="9475" max="9475" width="20.5546875" customWidth="1"/>
     <col min="9476" max="9476" width="17" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9479" max="9479" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="21.453125" customWidth="1"/>
-    <col min="9730" max="9730" width="14.81640625" customWidth="1"/>
-    <col min="9731" max="9731" width="20.54296875" customWidth="1"/>
+    <col min="9477" max="9477" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="21.44140625" customWidth="1"/>
+    <col min="9730" max="9730" width="14.77734375" customWidth="1"/>
+    <col min="9731" max="9731" width="20.5546875" customWidth="1"/>
     <col min="9732" max="9732" width="17" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9735" max="9735" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="21.453125" customWidth="1"/>
-    <col min="9986" max="9986" width="14.81640625" customWidth="1"/>
-    <col min="9987" max="9987" width="20.54296875" customWidth="1"/>
+    <col min="9733" max="9733" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="21.44140625" customWidth="1"/>
+    <col min="9986" max="9986" width="14.77734375" customWidth="1"/>
+    <col min="9987" max="9987" width="20.5546875" customWidth="1"/>
     <col min="9988" max="9988" width="17" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9991" max="9991" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="21.453125" customWidth="1"/>
-    <col min="10242" max="10242" width="14.81640625" customWidth="1"/>
-    <col min="10243" max="10243" width="20.54296875" customWidth="1"/>
+    <col min="9989" max="9989" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="21.44140625" customWidth="1"/>
+    <col min="10242" max="10242" width="14.77734375" customWidth="1"/>
+    <col min="10243" max="10243" width="20.5546875" customWidth="1"/>
     <col min="10244" max="10244" width="17" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10247" max="10247" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="21.453125" customWidth="1"/>
-    <col min="10498" max="10498" width="14.81640625" customWidth="1"/>
-    <col min="10499" max="10499" width="20.54296875" customWidth="1"/>
+    <col min="10245" max="10245" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="21.44140625" customWidth="1"/>
+    <col min="10498" max="10498" width="14.77734375" customWidth="1"/>
+    <col min="10499" max="10499" width="20.5546875" customWidth="1"/>
     <col min="10500" max="10500" width="17" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10503" max="10503" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="21.453125" customWidth="1"/>
-    <col min="10754" max="10754" width="14.81640625" customWidth="1"/>
-    <col min="10755" max="10755" width="20.54296875" customWidth="1"/>
+    <col min="10501" max="10501" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="21.44140625" customWidth="1"/>
+    <col min="10754" max="10754" width="14.77734375" customWidth="1"/>
+    <col min="10755" max="10755" width="20.5546875" customWidth="1"/>
     <col min="10756" max="10756" width="17" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10759" max="10759" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="21.453125" customWidth="1"/>
-    <col min="11010" max="11010" width="14.81640625" customWidth="1"/>
-    <col min="11011" max="11011" width="20.54296875" customWidth="1"/>
+    <col min="10757" max="10757" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="21.44140625" customWidth="1"/>
+    <col min="11010" max="11010" width="14.77734375" customWidth="1"/>
+    <col min="11011" max="11011" width="20.5546875" customWidth="1"/>
     <col min="11012" max="11012" width="17" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11015" max="11015" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="21.453125" customWidth="1"/>
-    <col min="11266" max="11266" width="14.81640625" customWidth="1"/>
-    <col min="11267" max="11267" width="20.54296875" customWidth="1"/>
+    <col min="11013" max="11013" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="21.44140625" customWidth="1"/>
+    <col min="11266" max="11266" width="14.77734375" customWidth="1"/>
+    <col min="11267" max="11267" width="20.5546875" customWidth="1"/>
     <col min="11268" max="11268" width="17" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11271" max="11271" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="21.453125" customWidth="1"/>
-    <col min="11522" max="11522" width="14.81640625" customWidth="1"/>
-    <col min="11523" max="11523" width="20.54296875" customWidth="1"/>
+    <col min="11269" max="11269" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="21.44140625" customWidth="1"/>
+    <col min="11522" max="11522" width="14.77734375" customWidth="1"/>
+    <col min="11523" max="11523" width="20.5546875" customWidth="1"/>
     <col min="11524" max="11524" width="17" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11527" max="11527" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="21.453125" customWidth="1"/>
-    <col min="11778" max="11778" width="14.81640625" customWidth="1"/>
-    <col min="11779" max="11779" width="20.54296875" customWidth="1"/>
+    <col min="11525" max="11525" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="21.44140625" customWidth="1"/>
+    <col min="11778" max="11778" width="14.77734375" customWidth="1"/>
+    <col min="11779" max="11779" width="20.5546875" customWidth="1"/>
     <col min="11780" max="11780" width="17" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11783" max="11783" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="21.453125" customWidth="1"/>
-    <col min="12034" max="12034" width="14.81640625" customWidth="1"/>
-    <col min="12035" max="12035" width="20.54296875" customWidth="1"/>
+    <col min="11781" max="11781" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="21.44140625" customWidth="1"/>
+    <col min="12034" max="12034" width="14.77734375" customWidth="1"/>
+    <col min="12035" max="12035" width="20.5546875" customWidth="1"/>
     <col min="12036" max="12036" width="17" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12039" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="21.453125" customWidth="1"/>
-    <col min="12290" max="12290" width="14.81640625" customWidth="1"/>
-    <col min="12291" max="12291" width="20.54296875" customWidth="1"/>
+    <col min="12037" max="12037" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="21.44140625" customWidth="1"/>
+    <col min="12290" max="12290" width="14.77734375" customWidth="1"/>
+    <col min="12291" max="12291" width="20.5546875" customWidth="1"/>
     <col min="12292" max="12292" width="17" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12295" max="12295" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="21.453125" customWidth="1"/>
-    <col min="12546" max="12546" width="14.81640625" customWidth="1"/>
-    <col min="12547" max="12547" width="20.54296875" customWidth="1"/>
+    <col min="12293" max="12293" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="21.44140625" customWidth="1"/>
+    <col min="12546" max="12546" width="14.77734375" customWidth="1"/>
+    <col min="12547" max="12547" width="20.5546875" customWidth="1"/>
     <col min="12548" max="12548" width="17" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12551" max="12551" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="21.453125" customWidth="1"/>
-    <col min="12802" max="12802" width="14.81640625" customWidth="1"/>
-    <col min="12803" max="12803" width="20.54296875" customWidth="1"/>
+    <col min="12549" max="12549" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="21.44140625" customWidth="1"/>
+    <col min="12802" max="12802" width="14.77734375" customWidth="1"/>
+    <col min="12803" max="12803" width="20.5546875" customWidth="1"/>
     <col min="12804" max="12804" width="17" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12807" max="12807" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="21.453125" customWidth="1"/>
-    <col min="13058" max="13058" width="14.81640625" customWidth="1"/>
-    <col min="13059" max="13059" width="20.54296875" customWidth="1"/>
+    <col min="12805" max="12805" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="21.44140625" customWidth="1"/>
+    <col min="13058" max="13058" width="14.77734375" customWidth="1"/>
+    <col min="13059" max="13059" width="20.5546875" customWidth="1"/>
     <col min="13060" max="13060" width="17" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13063" max="13063" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="21.453125" customWidth="1"/>
-    <col min="13314" max="13314" width="14.81640625" customWidth="1"/>
-    <col min="13315" max="13315" width="20.54296875" customWidth="1"/>
+    <col min="13061" max="13061" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="21.44140625" customWidth="1"/>
+    <col min="13314" max="13314" width="14.77734375" customWidth="1"/>
+    <col min="13315" max="13315" width="20.5546875" customWidth="1"/>
     <col min="13316" max="13316" width="17" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13319" max="13319" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="21.453125" customWidth="1"/>
-    <col min="13570" max="13570" width="14.81640625" customWidth="1"/>
-    <col min="13571" max="13571" width="20.54296875" customWidth="1"/>
+    <col min="13317" max="13317" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="21.44140625" customWidth="1"/>
+    <col min="13570" max="13570" width="14.77734375" customWidth="1"/>
+    <col min="13571" max="13571" width="20.5546875" customWidth="1"/>
     <col min="13572" max="13572" width="17" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13575" max="13575" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="21.453125" customWidth="1"/>
-    <col min="13826" max="13826" width="14.81640625" customWidth="1"/>
-    <col min="13827" max="13827" width="20.54296875" customWidth="1"/>
+    <col min="13573" max="13573" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="21.44140625" customWidth="1"/>
+    <col min="13826" max="13826" width="14.77734375" customWidth="1"/>
+    <col min="13827" max="13827" width="20.5546875" customWidth="1"/>
     <col min="13828" max="13828" width="17" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13831" max="13831" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="21.453125" customWidth="1"/>
-    <col min="14082" max="14082" width="14.81640625" customWidth="1"/>
-    <col min="14083" max="14083" width="20.54296875" customWidth="1"/>
+    <col min="13829" max="13829" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="21.44140625" customWidth="1"/>
+    <col min="14082" max="14082" width="14.77734375" customWidth="1"/>
+    <col min="14083" max="14083" width="20.5546875" customWidth="1"/>
     <col min="14084" max="14084" width="17" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14087" max="14087" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="21.453125" customWidth="1"/>
-    <col min="14338" max="14338" width="14.81640625" customWidth="1"/>
-    <col min="14339" max="14339" width="20.54296875" customWidth="1"/>
+    <col min="14085" max="14085" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="21.44140625" customWidth="1"/>
+    <col min="14338" max="14338" width="14.77734375" customWidth="1"/>
+    <col min="14339" max="14339" width="20.5546875" customWidth="1"/>
     <col min="14340" max="14340" width="17" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14343" max="14343" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="21.453125" customWidth="1"/>
-    <col min="14594" max="14594" width="14.81640625" customWidth="1"/>
-    <col min="14595" max="14595" width="20.54296875" customWidth="1"/>
+    <col min="14341" max="14341" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="21.44140625" customWidth="1"/>
+    <col min="14594" max="14594" width="14.77734375" customWidth="1"/>
+    <col min="14595" max="14595" width="20.5546875" customWidth="1"/>
     <col min="14596" max="14596" width="17" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14599" max="14599" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="21.453125" customWidth="1"/>
-    <col min="14850" max="14850" width="14.81640625" customWidth="1"/>
-    <col min="14851" max="14851" width="20.54296875" customWidth="1"/>
+    <col min="14597" max="14597" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="21.44140625" customWidth="1"/>
+    <col min="14850" max="14850" width="14.77734375" customWidth="1"/>
+    <col min="14851" max="14851" width="20.5546875" customWidth="1"/>
     <col min="14852" max="14852" width="17" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14855" max="14855" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="21.453125" customWidth="1"/>
-    <col min="15106" max="15106" width="14.81640625" customWidth="1"/>
-    <col min="15107" max="15107" width="20.54296875" customWidth="1"/>
+    <col min="14853" max="14853" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="21.44140625" customWidth="1"/>
+    <col min="15106" max="15106" width="14.77734375" customWidth="1"/>
+    <col min="15107" max="15107" width="20.5546875" customWidth="1"/>
     <col min="15108" max="15108" width="17" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15111" max="15111" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="21.453125" customWidth="1"/>
-    <col min="15362" max="15362" width="14.81640625" customWidth="1"/>
-    <col min="15363" max="15363" width="20.54296875" customWidth="1"/>
+    <col min="15109" max="15109" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="21.44140625" customWidth="1"/>
+    <col min="15362" max="15362" width="14.77734375" customWidth="1"/>
+    <col min="15363" max="15363" width="20.5546875" customWidth="1"/>
     <col min="15364" max="15364" width="17" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15367" max="15367" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="21.453125" customWidth="1"/>
-    <col min="15618" max="15618" width="14.81640625" customWidth="1"/>
-    <col min="15619" max="15619" width="20.54296875" customWidth="1"/>
+    <col min="15365" max="15365" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="21.44140625" customWidth="1"/>
+    <col min="15618" max="15618" width="14.77734375" customWidth="1"/>
+    <col min="15619" max="15619" width="20.5546875" customWidth="1"/>
     <col min="15620" max="15620" width="17" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15623" max="15623" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="21.453125" customWidth="1"/>
-    <col min="15874" max="15874" width="14.81640625" customWidth="1"/>
-    <col min="15875" max="15875" width="20.54296875" customWidth="1"/>
+    <col min="15621" max="15621" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="21.44140625" customWidth="1"/>
+    <col min="15874" max="15874" width="14.77734375" customWidth="1"/>
+    <col min="15875" max="15875" width="20.5546875" customWidth="1"/>
     <col min="15876" max="15876" width="17" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15879" max="15879" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="21.453125" customWidth="1"/>
-    <col min="16130" max="16130" width="14.81640625" customWidth="1"/>
-    <col min="16131" max="16131" width="20.54296875" customWidth="1"/>
+    <col min="15877" max="15877" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="21.44140625" customWidth="1"/>
+    <col min="16130" max="16130" width="14.77734375" customWidth="1"/>
+    <col min="16131" max="16131" width="20.5546875" customWidth="1"/>
     <col min="16132" max="16132" width="17" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="16135" max="16135" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11861,7 +11934,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>889</v>
       </c>
@@ -11890,7 +11963,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>895</v>
       </c>
@@ -11919,7 +11992,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>901</v>
       </c>
@@ -11949,7 +12022,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>889</v>
       </c>
@@ -11978,7 +12051,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>889</v>
       </c>
@@ -12007,7 +12080,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>889</v>
       </c>
@@ -12036,7 +12109,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>895</v>
       </c>
@@ -12065,7 +12138,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>921</v>
       </c>
@@ -12094,7 +12167,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>921</v>
       </c>
@@ -12142,26 +12215,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A03146-6FE6-45D1-B4C6-477159028F0E}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12214,7 +12287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -12252,7 +12325,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -12290,7 +12363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -12328,7 +12401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>610</v>
       </c>
@@ -12366,7 +12439,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>717</v>
       </c>
@@ -12404,7 +12477,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>731</v>
       </c>
@@ -12442,7 +12515,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>748</v>
       </c>
@@ -12480,7 +12553,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>753</v>
       </c>
@@ -12518,7 +12591,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>757</v>
       </c>
@@ -12556,7 +12629,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>879</v>
       </c>
@@ -12594,7 +12667,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>887</v>
       </c>
@@ -12632,7 +12705,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>942</v>
       </c>
@@ -12670,7 +12743,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>984</v>
       </c>
@@ -12708,7 +12781,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1001</v>
       </c>
@@ -12756,22 +12829,22 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12824,7 +12897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>744272121</v>
       </c>
@@ -12859,7 +12932,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>635</v>
       </c>
@@ -12897,7 +12970,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>701</v>
       </c>
@@ -12932,7 +13005,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>761</v>
       </c>
@@ -12970,7 +13043,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="28" ht="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" ht="13.35" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12985,9 +13058,9 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13007,7 +13080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>766</v>
       </c>
@@ -13040,18 +13113,18 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -13080,7 +13153,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>589</v>
       </c>
@@ -13109,7 +13182,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>589</v>
       </c>
@@ -13138,7 +13211,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>843</v>
       </c>
@@ -13183,21 +13256,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -13232,7 +13305,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>796</v>
       </c>
@@ -13267,7 +13340,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>792</v>
       </c>
@@ -13302,7 +13375,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>939</v>
       </c>
@@ -13354,21 +13427,21 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13415,7 +13488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>581</v>
       </c>
@@ -13447,7 +13520,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>603</v>
       </c>
@@ -13476,7 +13549,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>708</v>
       </c>
@@ -13508,7 +13581,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>830</v>
       </c>
@@ -13538,7 +13611,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>859</v>
       </c>
@@ -13581,14 +13654,14 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13629,7 +13702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>648</v>
       </c>
@@ -13660,7 +13733,7 @@
       <c r="U2" s="7"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>649</v>
       </c>
@@ -13691,7 +13764,7 @@
       <c r="U3" s="7"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>650</v>
       </c>
@@ -13722,7 +13795,7 @@
       <c r="U4" s="7"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>651</v>
       </c>
@@ -13753,7 +13826,7 @@
       <c r="U5" s="7"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>652</v>
       </c>
@@ -13784,11 +13857,11 @@
       <c r="U6" s="7"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E7" s="7"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E8" s="7"/>
       <c r="H8" s="5"/>
     </row>
@@ -13805,21 +13878,21 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13866,7 +13939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>595</v>
       </c>
@@ -13898,7 +13971,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>666</v>
       </c>
@@ -13930,7 +14003,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>865</v>
       </c>
@@ -13962,7 +14035,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>969</v>
       </c>
@@ -13994,7 +14067,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I9" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added High-Side Driver for PDM
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\refic\3D Objects\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AD0811-30C7-47D9-8DC4-36370D6F75FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972930E7-EF4F-4E71-886A-98E0D8745D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1545" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2798" uniqueCount="1023">
   <si>
     <t>Part Number</t>
   </si>
@@ -3107,6 +3107,21 @@
   </si>
   <si>
     <t>TE_SMF7</t>
+  </si>
+  <si>
+    <t>TPS1HTC30AQPWPRQ1</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE, 60-V, 6-A, 30-M, ONE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/texas-instruments/TPS1HTC30AQPWPRQ1/22106757</t>
+  </si>
+  <si>
+    <t>296-TPS1HTC30AQPWPRQ1TR-ND</t>
+  </si>
+  <si>
+    <t>TI_TSSOP</t>
   </si>
 </sst>
 </file>
@@ -3487,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I188" sqref="I188"/>
+    <sheetView topLeftCell="A183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10216,10 +10231,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10931,6 +10946,38 @@
         <v>35</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>563</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F24" t="s">
+        <v>570</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>1020</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{815BD2A1-6E8A-46F8-9861-C78A08FF1096}"/>
@@ -10940,9 +10987,10 @@
     <hyperlink ref="J7" r:id="rId5" xr:uid="{71439ED1-BAD7-46B8-9FA2-B26BCC099889}"/>
     <hyperlink ref="J9" r:id="rId6" xr:uid="{CD33C165-116A-4895-BF42-9E15D8C3F899}"/>
     <hyperlink ref="J16" r:id="rId7" xr:uid="{E0AFB124-543E-4E34-8464-CF1CC76A6806}"/>
+    <hyperlink ref="J24" r:id="rId8" xr:uid="{58A877EE-EF13-4EB4-94D6-60895FE71EE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Component Upload for PDM
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0B541-34BB-4AD3-B3B6-03A20C56BE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7D4749-C161-475E-A785-A31E6397A286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1036">
   <si>
     <t>Part Number</t>
   </si>
@@ -3134,6 +3134,33 @@
   </si>
   <si>
     <t>MMBZ5230BLT1GOSTR-ND</t>
+  </si>
+  <si>
+    <t>MSX1PJ-M3/89A</t>
+  </si>
+  <si>
+    <t>600V</t>
+  </si>
+  <si>
+    <t>VISHAY DO-219</t>
+  </si>
+  <si>
+    <t>GCM188R71H223KA37J</t>
+  </si>
+  <si>
+    <t>22nF</t>
+  </si>
+  <si>
+    <t>490-8022-2-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-7W24KL</t>
+  </si>
+  <si>
+    <t>0.2W</t>
+  </si>
+  <si>
+    <t>13-RC0603FR-7W24KL-ND</t>
   </si>
 </sst>
 </file>
@@ -3512,10 +3539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T186"/>
+  <dimension ref="A1:T187"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I188" sqref="I188"/>
+    <sheetView tabSelected="1" topLeftCell="B171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G188" sqref="G188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10231,6 +10258,38 @@
       </c>
       <c r="J186" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B187" t="s">
+        <v>55</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D187" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G187" t="s">
+        <v>726</v>
+      </c>
+      <c r="H187" t="s">
+        <v>33</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="J187" t="s">
+        <v>35</v>
+      </c>
+      <c r="M187" t="s">
+        <v>1035</v>
       </c>
     </row>
   </sheetData>
@@ -12301,10 +12360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A03146-6FE6-45D1-B4C6-477159028F0E}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12902,6 +12961,44 @@
       </c>
       <c r="K15" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B16" t="s">
+        <v>747</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>719</v>
+      </c>
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -13547,10 +13644,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB642537-4F8F-408B-8CD8-6454E1D4B8C7}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13822,6 +13919,29 @@
       </c>
       <c r="L8" t="s">
         <v>1026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B9" t="s">
+        <v>858</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F9" t="s">
+        <v>607</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATED WITH MY HSD!
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\refic\3D Objects\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E20C878-8264-4DC6-A690-E31810B1E5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC0CA60-ECC3-4246-AE53-B2C7F80550FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1545" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10320" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1050">
   <si>
     <t>Part Number</t>
   </si>
@@ -3188,6 +3188,21 @@
   </si>
   <si>
     <t>Onsemi_DPAK</t>
+  </si>
+  <si>
+    <t>TPS1HTC30AQPWPRQ1</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE, 60-V, 6-A, 30-M, ONE</t>
+  </si>
+  <si>
+    <t>TI_14_TSSOP</t>
+  </si>
+  <si>
+    <t>296-TPS1HTC30AQPWPRQ1TR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/texas-instruments/TPS1HTC30AQPWPRQ1/22106757</t>
   </si>
 </sst>
 </file>
@@ -10329,10 +10344,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11044,6 +11059,38 @@
         <v>35</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>563</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F24" t="s">
+        <v>570</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>1049</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{815BD2A1-6E8A-46F8-9861-C78A08FF1096}"/>
@@ -11053,9 +11100,10 @@
     <hyperlink ref="J7" r:id="rId5" xr:uid="{71439ED1-BAD7-46B8-9FA2-B26BCC099889}"/>
     <hyperlink ref="J9" r:id="rId6" xr:uid="{CD33C165-116A-4895-BF42-9E15D8C3F899}"/>
     <hyperlink ref="J16" r:id="rId7" xr:uid="{E0AFB124-543E-4E34-8464-CF1CC76A6806}"/>
+    <hyperlink ref="J24" r:id="rId8" xr:uid="{D74EC88D-B326-400E-884E-3D5C7C6838E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -11166,8 +11214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEF819E-36FD-41E5-A84F-246B77FC8D19}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updates and modifications of pad shapes
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\refic\3D Objects\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC0CA60-ECC3-4246-AE53-B2C7F80550FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B7240D-A075-4C0C-AF57-19EAF5EA4CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10320" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="1545" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="1051">
   <si>
     <t>Part Number</t>
   </si>
@@ -3203,6 +3203,9 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/en/products/detail/texas-instruments/TPS1HTC30AQPWPRQ1/22106757</t>
+  </si>
+  <si>
+    <t>3339P-1-1103LF</t>
   </si>
 </sst>
 </file>
@@ -3581,10 +3584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T187"/>
+  <dimension ref="A1:T188"/>
   <sheetViews>
-    <sheetView topLeftCell="B171" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G188" sqref="G188"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J191" sqref="J191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10334,6 +10337,35 @@
         <v>1035</v>
       </c>
     </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B188" t="s">
+        <v>679</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D188" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F188" t="s">
+        <v>681</v>
+      </c>
+      <c r="G188" t="s">
+        <v>682</v>
+      </c>
+      <c r="H188" t="s">
+        <v>33</v>
+      </c>
+      <c r="I188" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J188" t="s">
+        <v>579</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="I1:I185" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -10346,7 +10378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added some more components for use with the L9963E (for FYP BMS Remote Module)
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA331398-B5C9-4282-B02F-A66BA0172C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190DAB8-E84C-494E-AB2B-06F03CD363FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="1150">
   <si>
     <t>Part Number</t>
   </si>
@@ -3347,6 +3347,162 @@
   </si>
   <si>
     <t>2449-J104B2C12VDC.20S-ND</t>
+  </si>
+  <si>
+    <t>PS2703-1-F3</t>
+  </si>
+  <si>
+    <t>Renesas Electronics Corporation</t>
+  </si>
+  <si>
+    <t>OPTOISOLATOR 3.75KV TRANS 4SMD</t>
+  </si>
+  <si>
+    <t>PS2703-1-F3-A</t>
+  </si>
+  <si>
+    <t>4-SOP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/renesas-electronics-corporation/PS2703-1-F3-A/9564816</t>
+  </si>
+  <si>
+    <t>559-1155-6-ND</t>
+  </si>
+  <si>
+    <t>STS8DN6LF6AG</t>
+  </si>
+  <si>
+    <t>Mosfet Array 60V 8A (Ta) 3.2W Surface Mount 8-SO</t>
+  </si>
+  <si>
+    <t>497-17309-6-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/stmicro/STS8DN6LF6AG/7360928?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Low%20Performing%20Products&amp;utm_term=&amp;utm_id=go_cmp-20086482685_adg-_ad-__dev-c_ext-_prd-_sig-Cj0KCQjw-5y1BhC-ARIsAAM_oKlrWFJm59o1biWSy2EnzNrM1cX7uWe4kK_gel5nDG0YwSBSqr3wylYaAvjiEALw_wcB&amp;productid=&amp;utm_content=&amp;gad_source=1&amp;gclid=Cj0KCQjw-5y1BhC-ARIsAAM_oKlrWFJm59o1biWSy2EnzNrM1cX7uWe4kK_gel5nDG0YwSBSqr3wylYaAvjiEALw_wcB</t>
+  </si>
+  <si>
+    <t>SO-8_STM-M</t>
+  </si>
+  <si>
+    <t>CGA3E2X7R2A472K080AA</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>445-5810-6-ND</t>
+  </si>
+  <si>
+    <t>CRCW251247R0FKEG</t>
+  </si>
+  <si>
+    <t>541-47.0AFDKR-ND</t>
+  </si>
+  <si>
+    <t>Resistor 2512</t>
+  </si>
+  <si>
+    <t>Thick Film</t>
+  </si>
+  <si>
+    <t>C1210X475K101T</t>
+  </si>
+  <si>
+    <t>Holy Stone Enterprise Co., Ltd.</t>
+  </si>
+  <si>
+    <t>4587-C1210X475K101TDKR-ND</t>
+  </si>
+  <si>
+    <t>CL32B225KCJSNNE</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>1276-3362-6-ND</t>
+  </si>
+  <si>
+    <t>CL10B333KC8WPNC</t>
+  </si>
+  <si>
+    <t>33nF</t>
+  </si>
+  <si>
+    <t>1276-CL10B333KC8WPNCDKR-ND</t>
+  </si>
+  <si>
+    <t>CL10B104KC8NNNC</t>
+  </si>
+  <si>
+    <t>1276-6807-6-ND</t>
+  </si>
+  <si>
+    <t>Resistor 0612</t>
+  </si>
+  <si>
+    <t>0612</t>
+  </si>
+  <si>
+    <t>3430B2F3K9TDF</t>
+  </si>
+  <si>
+    <t>TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t>3.9K</t>
+  </si>
+  <si>
+    <t>1.5W</t>
+  </si>
+  <si>
+    <t>1712-3430B2F3K9TDFDKR-ND</t>
+  </si>
+  <si>
+    <t>RCS080510K0FKEA</t>
+  </si>
+  <si>
+    <t>541-2845-6-ND</t>
+  </si>
+  <si>
+    <t>RCS0805680RFKEA</t>
+  </si>
+  <si>
+    <t>541-10548-6-ND</t>
+  </si>
+  <si>
+    <t>TRANS_STL60P4LLF6</t>
+  </si>
+  <si>
+    <t>STL8N10LF3</t>
+  </si>
+  <si>
+    <t>N-Channel 100 V 20A (Tc) 4.3W (Ta), 70W (Tc) Surface Mount PowerFlat™ (5x6)</t>
+  </si>
+  <si>
+    <t>70W</t>
+  </si>
+  <si>
+    <t>497-13652-6-ND</t>
+  </si>
+  <si>
+    <t>BLM31KN102SH1L</t>
+  </si>
+  <si>
+    <t>490-16520-6-ND</t>
+  </si>
+  <si>
+    <t>VJ0603Y101KXBCW1BC</t>
+  </si>
+  <si>
+    <t>Vishay Vitramon</t>
+  </si>
+  <si>
+    <t>720-VJ0603Y101KXBCW1BCDKR-ND</t>
   </si>
 </sst>
 </file>
@@ -3728,25 +3884,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T191"/>
+  <dimension ref="A1:T196"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D197" sqref="D197"/>
+    <sheetView topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P196" sqref="P196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -3832,7 +3988,7 @@
       </c>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -3868,7 +4024,7 @@
       </c>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -3904,7 +4060,7 @@
       </c>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
@@ -3940,7 +4096,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -3976,7 +4132,7 @@
       </c>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4012,7 +4168,7 @@
       </c>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -4048,7 +4204,7 @@
       </c>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
@@ -4084,7 +4240,7 @@
       </c>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -4120,7 +4276,7 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -4156,7 +4312,7 @@
       </c>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -4192,7 +4348,7 @@
       </c>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -4228,7 +4384,7 @@
       </c>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -4264,7 +4420,7 @@
       </c>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -4300,7 +4456,7 @@
       </c>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -4336,7 +4492,7 @@
       </c>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>103</v>
       </c>
@@ -4372,7 +4528,7 @@
       </c>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
@@ -4408,7 +4564,7 @@
       </c>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -4444,7 +4600,7 @@
       </c>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -4480,7 +4636,7 @@
       </c>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>115</v>
       </c>
@@ -4516,7 +4672,7 @@
       </c>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
@@ -4552,7 +4708,7 @@
       </c>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -4588,7 +4744,7 @@
       </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>124</v>
       </c>
@@ -4624,7 +4780,7 @@
       </c>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -4660,7 +4816,7 @@
       </c>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
@@ -4696,7 +4852,7 @@
       </c>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>133</v>
       </c>
@@ -4732,7 +4888,7 @@
       </c>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -4768,7 +4924,7 @@
       </c>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
@@ -4804,7 +4960,7 @@
       </c>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>142</v>
       </c>
@@ -4840,7 +4996,7 @@
       </c>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
@@ -4876,7 +5032,7 @@
       </c>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>148</v>
       </c>
@@ -4912,7 +5068,7 @@
       </c>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
@@ -4948,7 +5104,7 @@
       </c>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -4984,7 +5140,7 @@
       </c>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>157</v>
       </c>
@@ -5020,7 +5176,7 @@
       </c>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -5056,7 +5212,7 @@
       </c>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -5092,7 +5248,7 @@
       </c>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>166</v>
       </c>
@@ -5128,7 +5284,7 @@
       </c>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>169</v>
       </c>
@@ -5164,7 +5320,7 @@
       </c>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>172</v>
       </c>
@@ -5200,7 +5356,7 @@
       </c>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>175</v>
       </c>
@@ -5236,7 +5392,7 @@
       </c>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>178</v>
       </c>
@@ -5272,7 +5428,7 @@
       </c>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>181</v>
       </c>
@@ -5308,7 +5464,7 @@
       </c>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>184</v>
       </c>
@@ -5344,7 +5500,7 @@
       </c>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>187</v>
       </c>
@@ -5380,7 +5536,7 @@
       </c>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>190</v>
       </c>
@@ -5416,7 +5572,7 @@
       </c>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>193</v>
       </c>
@@ -5452,7 +5608,7 @@
       </c>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>196</v>
       </c>
@@ -5488,7 +5644,7 @@
       </c>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>199</v>
       </c>
@@ -5524,7 +5680,7 @@
       </c>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>202</v>
       </c>
@@ -5560,7 +5716,7 @@
       </c>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>205</v>
       </c>
@@ -5596,7 +5752,7 @@
       </c>
       <c r="T51" s="1"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>208</v>
       </c>
@@ -5632,7 +5788,7 @@
       </c>
       <c r="T52" s="1"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>211</v>
       </c>
@@ -5668,7 +5824,7 @@
       </c>
       <c r="T53" s="1"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>214</v>
       </c>
@@ -5704,7 +5860,7 @@
       </c>
       <c r="T54" s="1"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>217</v>
       </c>
@@ -5740,7 +5896,7 @@
       </c>
       <c r="T55" s="1"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>220</v>
       </c>
@@ -5776,7 +5932,7 @@
       </c>
       <c r="T56" s="1"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>223</v>
       </c>
@@ -5812,7 +5968,7 @@
       </c>
       <c r="T57" s="1"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -5848,7 +6004,7 @@
       </c>
       <c r="T58" s="1"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>228</v>
       </c>
@@ -5884,7 +6040,7 @@
       </c>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>231</v>
       </c>
@@ -5920,7 +6076,7 @@
       </c>
       <c r="T60" s="1"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
@@ -5956,7 +6112,7 @@
       </c>
       <c r="T61" s="1"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>237</v>
       </c>
@@ -5992,7 +6148,7 @@
       </c>
       <c r="T62" s="1"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>240</v>
       </c>
@@ -6028,7 +6184,7 @@
       </c>
       <c r="T63" s="1"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>243</v>
       </c>
@@ -6064,7 +6220,7 @@
       </c>
       <c r="T64" s="1"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>246</v>
       </c>
@@ -6100,7 +6256,7 @@
       </c>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>249</v>
       </c>
@@ -6136,7 +6292,7 @@
       </c>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>252</v>
       </c>
@@ -6172,7 +6328,7 @@
       </c>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>255</v>
       </c>
@@ -6208,7 +6364,7 @@
       </c>
       <c r="T68" s="1"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>258</v>
       </c>
@@ -6244,7 +6400,7 @@
       </c>
       <c r="T69" s="1"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>261</v>
       </c>
@@ -6280,7 +6436,7 @@
       </c>
       <c r="T70" s="1"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>264</v>
       </c>
@@ -6316,7 +6472,7 @@
       </c>
       <c r="T71" s="1"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>267</v>
       </c>
@@ -6352,7 +6508,7 @@
       </c>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>270</v>
       </c>
@@ -6388,7 +6544,7 @@
       </c>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>273</v>
       </c>
@@ -6424,7 +6580,7 @@
       </c>
       <c r="T74" s="1"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>276</v>
       </c>
@@ -6460,7 +6616,7 @@
       </c>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>279</v>
       </c>
@@ -6496,7 +6652,7 @@
       </c>
       <c r="T76" s="1"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6532,7 +6688,7 @@
       </c>
       <c r="T77" s="1"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6568,7 +6724,7 @@
       </c>
       <c r="T78" s="1"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>288</v>
       </c>
@@ -6604,7 +6760,7 @@
       </c>
       <c r="T79" s="1"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>291</v>
       </c>
@@ -6640,7 +6796,7 @@
       </c>
       <c r="T80" s="1"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>294</v>
       </c>
@@ -6676,7 +6832,7 @@
       </c>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>297</v>
       </c>
@@ -6712,7 +6868,7 @@
       </c>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>300</v>
       </c>
@@ -6748,7 +6904,7 @@
       </c>
       <c r="T83" s="1"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>303</v>
       </c>
@@ -6784,7 +6940,7 @@
       </c>
       <c r="T84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>306</v>
       </c>
@@ -6820,7 +6976,7 @@
       </c>
       <c r="T85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>309</v>
       </c>
@@ -6856,7 +7012,7 @@
       </c>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>312</v>
       </c>
@@ -6892,7 +7048,7 @@
       </c>
       <c r="T87" s="1"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>315</v>
       </c>
@@ -6928,7 +7084,7 @@
       </c>
       <c r="T88" s="1"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>318</v>
       </c>
@@ -6964,7 +7120,7 @@
       </c>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>321</v>
       </c>
@@ -7000,7 +7156,7 @@
       </c>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>324</v>
       </c>
@@ -7036,7 +7192,7 @@
       </c>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>327</v>
       </c>
@@ -7072,7 +7228,7 @@
       </c>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>330</v>
       </c>
@@ -7108,7 +7264,7 @@
       </c>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>333</v>
       </c>
@@ -7144,7 +7300,7 @@
       </c>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>336</v>
       </c>
@@ -7180,7 +7336,7 @@
       </c>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>339</v>
       </c>
@@ -7216,7 +7372,7 @@
       </c>
       <c r="T96" s="1"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>342</v>
       </c>
@@ -7252,7 +7408,7 @@
       </c>
       <c r="T97" s="1"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>345</v>
       </c>
@@ -7288,7 +7444,7 @@
       </c>
       <c r="T98" s="1"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>348</v>
       </c>
@@ -7324,7 +7480,7 @@
       </c>
       <c r="T99" s="1"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>351</v>
       </c>
@@ -7360,7 +7516,7 @@
       </c>
       <c r="T100" s="1"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>354</v>
       </c>
@@ -7396,7 +7552,7 @@
       </c>
       <c r="T101" s="1"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>357</v>
       </c>
@@ -7432,7 +7588,7 @@
       </c>
       <c r="T102" s="1"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>360</v>
       </c>
@@ -7468,7 +7624,7 @@
       </c>
       <c r="T103" s="1"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>363</v>
       </c>
@@ -7504,7 +7660,7 @@
       </c>
       <c r="T104" s="1"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>366</v>
       </c>
@@ -7540,7 +7696,7 @@
       </c>
       <c r="T105" s="1"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>369</v>
       </c>
@@ -7576,7 +7732,7 @@
       </c>
       <c r="T106" s="1"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>372</v>
       </c>
@@ -7612,7 +7768,7 @@
       </c>
       <c r="T107" s="1"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>375</v>
       </c>
@@ -7648,7 +7804,7 @@
       </c>
       <c r="T108" s="1"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>378</v>
       </c>
@@ -7684,7 +7840,7 @@
       </c>
       <c r="T109" s="1"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>381</v>
       </c>
@@ -7720,7 +7876,7 @@
       </c>
       <c r="T110" s="1"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>384</v>
       </c>
@@ -7756,7 +7912,7 @@
       </c>
       <c r="T111" s="1"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>387</v>
       </c>
@@ -7792,7 +7948,7 @@
       </c>
       <c r="T112" s="1"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>390</v>
       </c>
@@ -7828,7 +7984,7 @@
       </c>
       <c r="T113" s="1"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>393</v>
       </c>
@@ -7864,7 +8020,7 @@
       </c>
       <c r="T114" s="1"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>396</v>
       </c>
@@ -7900,7 +8056,7 @@
       </c>
       <c r="T115" s="1"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>399</v>
       </c>
@@ -7936,7 +8092,7 @@
       </c>
       <c r="T116" s="1"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>402</v>
       </c>
@@ -7972,7 +8128,7 @@
       </c>
       <c r="T117" s="1"/>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>402</v>
       </c>
@@ -8008,7 +8164,7 @@
       </c>
       <c r="T118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>407</v>
       </c>
@@ -8044,7 +8200,7 @@
       </c>
       <c r="T119" s="1"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>410</v>
       </c>
@@ -8080,7 +8236,7 @@
       </c>
       <c r="T120" s="1"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>413</v>
       </c>
@@ -8116,7 +8272,7 @@
       </c>
       <c r="T121" s="1"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>416</v>
       </c>
@@ -8153,7 +8309,7 @@
       </c>
       <c r="T122" s="1"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>419</v>
       </c>
@@ -8190,7 +8346,7 @@
       </c>
       <c r="T123" s="1"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>422</v>
       </c>
@@ -8227,7 +8383,7 @@
       </c>
       <c r="T124" s="1"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>424</v>
       </c>
@@ -8264,7 +8420,7 @@
       </c>
       <c r="T125" s="1"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>427</v>
       </c>
@@ -8301,7 +8457,7 @@
       </c>
       <c r="T126" s="1"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>430</v>
       </c>
@@ -8338,7 +8494,7 @@
       </c>
       <c r="T127" s="1"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>433</v>
       </c>
@@ -8375,7 +8531,7 @@
       </c>
       <c r="T128" s="1"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>436</v>
       </c>
@@ -8412,7 +8568,7 @@
       </c>
       <c r="T129" s="1"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>439</v>
       </c>
@@ -8449,7 +8605,7 @@
       </c>
       <c r="T130" s="1"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>442</v>
       </c>
@@ -8486,7 +8642,7 @@
       </c>
       <c r="T131" s="1"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>445</v>
       </c>
@@ -8523,7 +8679,7 @@
       </c>
       <c r="T132" s="1"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>448</v>
       </c>
@@ -8560,7 +8716,7 @@
       </c>
       <c r="T133" s="1"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>451</v>
       </c>
@@ -8597,7 +8753,7 @@
       </c>
       <c r="T134" s="1"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>454</v>
       </c>
@@ -8634,7 +8790,7 @@
       </c>
       <c r="T135" s="1"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>457</v>
       </c>
@@ -8671,7 +8827,7 @@
       </c>
       <c r="T136" s="1"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>460</v>
       </c>
@@ -8708,7 +8864,7 @@
       </c>
       <c r="T137" s="1"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>463</v>
       </c>
@@ -8745,7 +8901,7 @@
       </c>
       <c r="T138" s="1"/>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>466</v>
       </c>
@@ -8782,7 +8938,7 @@
       </c>
       <c r="T139" s="1"/>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>469</v>
       </c>
@@ -8819,7 +8975,7 @@
       </c>
       <c r="T140" s="1"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>472</v>
       </c>
@@ -8856,7 +9012,7 @@
       </c>
       <c r="T141" s="1"/>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>475</v>
       </c>
@@ -8893,7 +9049,7 @@
       </c>
       <c r="T142" s="1"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>478</v>
       </c>
@@ -8930,7 +9086,7 @@
       </c>
       <c r="T143" s="1"/>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>481</v>
       </c>
@@ -8967,7 +9123,7 @@
       </c>
       <c r="T144" s="1"/>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>484</v>
       </c>
@@ -9004,7 +9160,7 @@
       </c>
       <c r="T145" s="1"/>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>487</v>
       </c>
@@ -9040,7 +9196,7 @@
       </c>
       <c r="T146" s="1"/>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>490</v>
       </c>
@@ -9076,7 +9232,7 @@
       </c>
       <c r="T147" s="1"/>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>493</v>
       </c>
@@ -9112,7 +9268,7 @@
       </c>
       <c r="T148" s="1"/>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>496</v>
       </c>
@@ -9148,7 +9304,7 @@
       </c>
       <c r="T149" s="1"/>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>499</v>
       </c>
@@ -9184,7 +9340,7 @@
       </c>
       <c r="T150" s="1"/>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>502</v>
       </c>
@@ -9220,7 +9376,7 @@
       </c>
       <c r="T151" s="1"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>505</v>
       </c>
@@ -9256,7 +9412,7 @@
       </c>
       <c r="T152" s="1"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>508</v>
       </c>
@@ -9292,7 +9448,7 @@
       </c>
       <c r="T153" s="1"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>511</v>
       </c>
@@ -9328,7 +9484,7 @@
       </c>
       <c r="T154" s="1"/>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>514</v>
       </c>
@@ -9364,7 +9520,7 @@
       </c>
       <c r="T155" s="1"/>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>517</v>
       </c>
@@ -9400,7 +9556,7 @@
       </c>
       <c r="T156" s="1"/>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>520</v>
       </c>
@@ -9436,7 +9592,7 @@
       </c>
       <c r="T157" s="1"/>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>523</v>
       </c>
@@ -9472,7 +9628,7 @@
       </c>
       <c r="T158" s="1"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>526</v>
       </c>
@@ -9508,7 +9664,7 @@
       </c>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>529</v>
       </c>
@@ -9544,7 +9700,7 @@
       </c>
       <c r="T160" s="1"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>532</v>
       </c>
@@ -9580,7 +9736,7 @@
       </c>
       <c r="T161" s="1"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>535</v>
       </c>
@@ -9616,7 +9772,7 @@
       </c>
       <c r="T162" s="1"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>538</v>
       </c>
@@ -9652,7 +9808,7 @@
       </c>
       <c r="T163" s="1"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>541</v>
       </c>
@@ -9688,7 +9844,7 @@
       </c>
       <c r="T164" s="1"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>544</v>
       </c>
@@ -9724,7 +9880,7 @@
       </c>
       <c r="T165" s="1"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>547</v>
       </c>
@@ -9760,7 +9916,7 @@
       </c>
       <c r="T166" s="1"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>550</v>
       </c>
@@ -9796,7 +9952,7 @@
       </c>
       <c r="T167" s="1"/>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>553</v>
       </c>
@@ -9832,7 +9988,7 @@
       </c>
       <c r="T168" s="1"/>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>556</v>
       </c>
@@ -9868,7 +10024,7 @@
       </c>
       <c r="T169" s="1"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>559</v>
       </c>
@@ -9904,7 +10060,7 @@
       </c>
       <c r="T170" s="1"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>678</v>
       </c>
@@ -9936,7 +10092,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>733</v>
       </c>
@@ -9971,7 +10127,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>723</v>
       </c>
@@ -10006,7 +10162,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>735</v>
       </c>
@@ -10041,7 +10197,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>730</v>
       </c>
@@ -10076,7 +10232,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>851</v>
       </c>
@@ -10108,7 +10264,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>873</v>
       </c>
@@ -10143,7 +10299,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>929</v>
       </c>
@@ -10178,7 +10334,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>933</v>
       </c>
@@ -10213,7 +10369,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>936</v>
       </c>
@@ -10248,7 +10404,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>942</v>
       </c>
@@ -10280,7 +10436,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>943</v>
       </c>
@@ -10312,7 +10468,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>956</v>
       </c>
@@ -10347,7 +10503,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>969</v>
       </c>
@@ -10382,7 +10538,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>971</v>
       </c>
@@ -10417,7 +10573,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>1002</v>
       </c>
@@ -10449,7 +10605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>1022</v>
       </c>
@@ -10481,7 +10637,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>1039</v>
       </c>
@@ -10510,7 +10666,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>1049</v>
       </c>
@@ -10542,7 +10698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>1069</v>
       </c>
@@ -10568,7 +10724,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>1078</v>
       </c>
@@ -10598,6 +10754,175 @@
       </c>
       <c r="M191" t="s">
         <v>1082</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B192" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D192" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E192" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F192" t="s">
+        <v>946</v>
+      </c>
+      <c r="G192" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H192" t="s">
+        <v>33</v>
+      </c>
+      <c r="I192" s="1">
+        <v>2512</v>
+      </c>
+      <c r="J192" t="s">
+        <v>35</v>
+      </c>
+      <c r="M192" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D193" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E193" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G193" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H193" t="s">
+        <v>33</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J193" t="s">
+        <v>35</v>
+      </c>
+      <c r="M193" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="D194" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E194" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F194">
+        <v>0.5</v>
+      </c>
+      <c r="G194" t="s">
+        <v>722</v>
+      </c>
+      <c r="H194" t="s">
+        <v>33</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J194" t="s">
+        <v>35</v>
+      </c>
+      <c r="M194" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B195" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D195" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E195" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F195">
+        <v>0.5</v>
+      </c>
+      <c r="G195" t="s">
+        <v>722</v>
+      </c>
+      <c r="H195" t="s">
+        <v>33</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J195" t="s">
+        <v>35</v>
+      </c>
+      <c r="M195" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B196" t="s">
+        <v>747</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G196" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H196" t="s">
+        <v>33</v>
+      </c>
+      <c r="I196" s="12">
+        <v>1206</v>
+      </c>
+      <c r="J196" t="s">
+        <v>35</v>
+      </c>
+      <c r="M196" t="s">
+        <v>1146</v>
       </c>
     </row>
   </sheetData>
@@ -10610,27 +10935,27 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="98.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" customWidth="1"/>
-    <col min="7" max="7" width="21.453125" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="148" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10663,7 +10988,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>582</v>
       </c>
@@ -10695,7 +11020,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>689</v>
       </c>
@@ -10727,7 +11052,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>695</v>
       </c>
@@ -10759,7 +11084,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>774</v>
       </c>
@@ -10791,7 +11116,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>780</v>
       </c>
@@ -10823,7 +11148,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>582</v>
       </c>
@@ -10855,7 +11180,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>774</v>
       </c>
@@ -10887,7 +11212,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>737</v>
       </c>
@@ -10919,7 +11244,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>774</v>
       </c>
@@ -10951,7 +11276,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>737</v>
       </c>
@@ -10983,7 +11308,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>563</v>
       </c>
@@ -11015,7 +11340,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>924</v>
       </c>
@@ -11047,7 +11372,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>563</v>
       </c>
@@ -11073,7 +11398,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>563</v>
       </c>
@@ -11102,7 +11427,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>689</v>
       </c>
@@ -11134,7 +11459,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>689</v>
       </c>
@@ -11160,7 +11485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>563</v>
       </c>
@@ -11189,7 +11514,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>563</v>
       </c>
@@ -11221,7 +11546,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>737</v>
       </c>
@@ -11247,7 +11572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>689</v>
       </c>
@@ -11273,7 +11598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>689</v>
       </c>
@@ -11299,7 +11624,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>689</v>
       </c>
@@ -11325,7 +11650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>563</v>
       </c>
@@ -11357,7 +11682,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>563</v>
       </c>
@@ -11383,7 +11708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>563</v>
       </c>
@@ -11409,7 +11734,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1068</v>
       </c>
@@ -11435,7 +11760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>924</v>
       </c>
@@ -11459,6 +11784,70 @@
       </c>
       <c r="H28" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F29" t="s">
+        <v>570</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1104</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>582</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>570</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1108</v>
       </c>
     </row>
   </sheetData>
@@ -11485,18 +11874,18 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11543,7 +11932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>672</v>
       </c>
@@ -11584,527 +11973,527 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3A536-13FE-4779-967C-70D0B3D14BF0}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="21.453125" customWidth="1"/>
-    <col min="258" max="258" width="14.81640625" customWidth="1"/>
-    <col min="259" max="259" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="21.42578125" customWidth="1"/>
+    <col min="258" max="258" width="14.85546875" customWidth="1"/>
+    <col min="259" max="259" width="20.5703125" customWidth="1"/>
     <col min="260" max="260" width="17" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="21.453125" customWidth="1"/>
-    <col min="514" max="514" width="14.81640625" customWidth="1"/>
-    <col min="515" max="515" width="20.54296875" customWidth="1"/>
+    <col min="261" max="261" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="21.42578125" customWidth="1"/>
+    <col min="514" max="514" width="14.85546875" customWidth="1"/>
+    <col min="515" max="515" width="20.5703125" customWidth="1"/>
     <col min="516" max="516" width="17" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="21.453125" customWidth="1"/>
-    <col min="770" max="770" width="14.81640625" customWidth="1"/>
-    <col min="771" max="771" width="20.54296875" customWidth="1"/>
+    <col min="517" max="517" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="21.42578125" customWidth="1"/>
+    <col min="770" max="770" width="14.85546875" customWidth="1"/>
+    <col min="771" max="771" width="20.5703125" customWidth="1"/>
     <col min="772" max="772" width="17" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="775" max="775" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="21.453125" customWidth="1"/>
-    <col min="1026" max="1026" width="14.81640625" customWidth="1"/>
-    <col min="1027" max="1027" width="20.54296875" customWidth="1"/>
+    <col min="773" max="773" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="21.42578125" customWidth="1"/>
+    <col min="1026" max="1026" width="14.85546875" customWidth="1"/>
+    <col min="1027" max="1027" width="20.5703125" customWidth="1"/>
     <col min="1028" max="1028" width="17" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1031" max="1031" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="21.453125" customWidth="1"/>
-    <col min="1282" max="1282" width="14.81640625" customWidth="1"/>
-    <col min="1283" max="1283" width="20.54296875" customWidth="1"/>
+    <col min="1029" max="1029" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="21.42578125" customWidth="1"/>
+    <col min="1282" max="1282" width="14.85546875" customWidth="1"/>
+    <col min="1283" max="1283" width="20.5703125" customWidth="1"/>
     <col min="1284" max="1284" width="17" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1287" max="1287" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="21.453125" customWidth="1"/>
-    <col min="1538" max="1538" width="14.81640625" customWidth="1"/>
-    <col min="1539" max="1539" width="20.54296875" customWidth="1"/>
+    <col min="1285" max="1285" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="21.42578125" customWidth="1"/>
+    <col min="1538" max="1538" width="14.85546875" customWidth="1"/>
+    <col min="1539" max="1539" width="20.5703125" customWidth="1"/>
     <col min="1540" max="1540" width="17" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1543" max="1543" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="21.453125" customWidth="1"/>
-    <col min="1794" max="1794" width="14.81640625" customWidth="1"/>
-    <col min="1795" max="1795" width="20.54296875" customWidth="1"/>
+    <col min="1541" max="1541" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="21.42578125" customWidth="1"/>
+    <col min="1794" max="1794" width="14.85546875" customWidth="1"/>
+    <col min="1795" max="1795" width="20.5703125" customWidth="1"/>
     <col min="1796" max="1796" width="17" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="1799" max="1799" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="21.453125" customWidth="1"/>
-    <col min="2050" max="2050" width="14.81640625" customWidth="1"/>
-    <col min="2051" max="2051" width="20.54296875" customWidth="1"/>
+    <col min="1797" max="1797" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="21.42578125" customWidth="1"/>
+    <col min="2050" max="2050" width="14.85546875" customWidth="1"/>
+    <col min="2051" max="2051" width="20.5703125" customWidth="1"/>
     <col min="2052" max="2052" width="17" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2055" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="21.453125" customWidth="1"/>
-    <col min="2306" max="2306" width="14.81640625" customWidth="1"/>
-    <col min="2307" max="2307" width="20.54296875" customWidth="1"/>
+    <col min="2053" max="2053" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="21.42578125" customWidth="1"/>
+    <col min="2306" max="2306" width="14.85546875" customWidth="1"/>
+    <col min="2307" max="2307" width="20.5703125" customWidth="1"/>
     <col min="2308" max="2308" width="17" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2311" max="2311" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="21.453125" customWidth="1"/>
-    <col min="2562" max="2562" width="14.81640625" customWidth="1"/>
-    <col min="2563" max="2563" width="20.54296875" customWidth="1"/>
+    <col min="2309" max="2309" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="21.42578125" customWidth="1"/>
+    <col min="2562" max="2562" width="14.85546875" customWidth="1"/>
+    <col min="2563" max="2563" width="20.5703125" customWidth="1"/>
     <col min="2564" max="2564" width="17" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2567" max="2567" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="21.453125" customWidth="1"/>
-    <col min="2818" max="2818" width="14.81640625" customWidth="1"/>
-    <col min="2819" max="2819" width="20.54296875" customWidth="1"/>
+    <col min="2565" max="2565" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="21.42578125" customWidth="1"/>
+    <col min="2818" max="2818" width="14.85546875" customWidth="1"/>
+    <col min="2819" max="2819" width="20.5703125" customWidth="1"/>
     <col min="2820" max="2820" width="17" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2823" max="2823" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="21.453125" customWidth="1"/>
-    <col min="3074" max="3074" width="14.81640625" customWidth="1"/>
-    <col min="3075" max="3075" width="20.54296875" customWidth="1"/>
+    <col min="2821" max="2821" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="21.42578125" customWidth="1"/>
+    <col min="3074" max="3074" width="14.85546875" customWidth="1"/>
+    <col min="3075" max="3075" width="20.5703125" customWidth="1"/>
     <col min="3076" max="3076" width="17" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3079" max="3079" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="21.453125" customWidth="1"/>
-    <col min="3330" max="3330" width="14.81640625" customWidth="1"/>
-    <col min="3331" max="3331" width="20.54296875" customWidth="1"/>
+    <col min="3077" max="3077" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="21.42578125" customWidth="1"/>
+    <col min="3330" max="3330" width="14.85546875" customWidth="1"/>
+    <col min="3331" max="3331" width="20.5703125" customWidth="1"/>
     <col min="3332" max="3332" width="17" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3335" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="21.453125" customWidth="1"/>
-    <col min="3586" max="3586" width="14.81640625" customWidth="1"/>
-    <col min="3587" max="3587" width="20.54296875" customWidth="1"/>
+    <col min="3333" max="3333" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="21.42578125" customWidth="1"/>
+    <col min="3586" max="3586" width="14.85546875" customWidth="1"/>
+    <col min="3587" max="3587" width="20.5703125" customWidth="1"/>
     <col min="3588" max="3588" width="17" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3591" max="3591" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="21.453125" customWidth="1"/>
-    <col min="3842" max="3842" width="14.81640625" customWidth="1"/>
-    <col min="3843" max="3843" width="20.54296875" customWidth="1"/>
+    <col min="3589" max="3589" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="21.42578125" customWidth="1"/>
+    <col min="3842" max="3842" width="14.85546875" customWidth="1"/>
+    <col min="3843" max="3843" width="20.5703125" customWidth="1"/>
     <col min="3844" max="3844" width="17" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3847" max="3847" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="21.453125" customWidth="1"/>
-    <col min="4098" max="4098" width="14.81640625" customWidth="1"/>
-    <col min="4099" max="4099" width="20.54296875" customWidth="1"/>
+    <col min="3845" max="3845" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="21.42578125" customWidth="1"/>
+    <col min="4098" max="4098" width="14.85546875" customWidth="1"/>
+    <col min="4099" max="4099" width="20.5703125" customWidth="1"/>
     <col min="4100" max="4100" width="17" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4103" max="4103" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="21.453125" customWidth="1"/>
-    <col min="4354" max="4354" width="14.81640625" customWidth="1"/>
-    <col min="4355" max="4355" width="20.54296875" customWidth="1"/>
+    <col min="4101" max="4101" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="21.42578125" customWidth="1"/>
+    <col min="4354" max="4354" width="14.85546875" customWidth="1"/>
+    <col min="4355" max="4355" width="20.5703125" customWidth="1"/>
     <col min="4356" max="4356" width="17" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4359" max="4359" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="21.453125" customWidth="1"/>
-    <col min="4610" max="4610" width="14.81640625" customWidth="1"/>
-    <col min="4611" max="4611" width="20.54296875" customWidth="1"/>
+    <col min="4357" max="4357" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="21.42578125" customWidth="1"/>
+    <col min="4610" max="4610" width="14.85546875" customWidth="1"/>
+    <col min="4611" max="4611" width="20.5703125" customWidth="1"/>
     <col min="4612" max="4612" width="17" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4615" max="4615" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="21.453125" customWidth="1"/>
-    <col min="4866" max="4866" width="14.81640625" customWidth="1"/>
-    <col min="4867" max="4867" width="20.54296875" customWidth="1"/>
+    <col min="4613" max="4613" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="21.42578125" customWidth="1"/>
+    <col min="4866" max="4866" width="14.85546875" customWidth="1"/>
+    <col min="4867" max="4867" width="20.5703125" customWidth="1"/>
     <col min="4868" max="4868" width="17" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4871" max="4871" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="21.453125" customWidth="1"/>
-    <col min="5122" max="5122" width="14.81640625" customWidth="1"/>
-    <col min="5123" max="5123" width="20.54296875" customWidth="1"/>
+    <col min="4869" max="4869" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="21.42578125" customWidth="1"/>
+    <col min="5122" max="5122" width="14.85546875" customWidth="1"/>
+    <col min="5123" max="5123" width="20.5703125" customWidth="1"/>
     <col min="5124" max="5124" width="17" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5127" max="5127" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="21.453125" customWidth="1"/>
-    <col min="5378" max="5378" width="14.81640625" customWidth="1"/>
-    <col min="5379" max="5379" width="20.54296875" customWidth="1"/>
+    <col min="5125" max="5125" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="21.42578125" customWidth="1"/>
+    <col min="5378" max="5378" width="14.85546875" customWidth="1"/>
+    <col min="5379" max="5379" width="20.5703125" customWidth="1"/>
     <col min="5380" max="5380" width="17" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5383" max="5383" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="21.453125" customWidth="1"/>
-    <col min="5634" max="5634" width="14.81640625" customWidth="1"/>
-    <col min="5635" max="5635" width="20.54296875" customWidth="1"/>
+    <col min="5381" max="5381" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="21.42578125" customWidth="1"/>
+    <col min="5634" max="5634" width="14.85546875" customWidth="1"/>
+    <col min="5635" max="5635" width="20.5703125" customWidth="1"/>
     <col min="5636" max="5636" width="17" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5639" max="5639" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="21.453125" customWidth="1"/>
-    <col min="5890" max="5890" width="14.81640625" customWidth="1"/>
-    <col min="5891" max="5891" width="20.54296875" customWidth="1"/>
+    <col min="5637" max="5637" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="21.42578125" customWidth="1"/>
+    <col min="5890" max="5890" width="14.85546875" customWidth="1"/>
+    <col min="5891" max="5891" width="20.5703125" customWidth="1"/>
     <col min="5892" max="5892" width="17" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5895" max="5895" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="21.453125" customWidth="1"/>
-    <col min="6146" max="6146" width="14.81640625" customWidth="1"/>
-    <col min="6147" max="6147" width="20.54296875" customWidth="1"/>
+    <col min="5893" max="5893" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="21.42578125" customWidth="1"/>
+    <col min="6146" max="6146" width="14.85546875" customWidth="1"/>
+    <col min="6147" max="6147" width="20.5703125" customWidth="1"/>
     <col min="6148" max="6148" width="17" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6151" max="6151" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="21.453125" customWidth="1"/>
-    <col min="6402" max="6402" width="14.81640625" customWidth="1"/>
-    <col min="6403" max="6403" width="20.54296875" customWidth="1"/>
+    <col min="6149" max="6149" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="21.42578125" customWidth="1"/>
+    <col min="6402" max="6402" width="14.85546875" customWidth="1"/>
+    <col min="6403" max="6403" width="20.5703125" customWidth="1"/>
     <col min="6404" max="6404" width="17" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6407" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="21.453125" customWidth="1"/>
-    <col min="6658" max="6658" width="14.81640625" customWidth="1"/>
-    <col min="6659" max="6659" width="20.54296875" customWidth="1"/>
+    <col min="6405" max="6405" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="21.42578125" customWidth="1"/>
+    <col min="6658" max="6658" width="14.85546875" customWidth="1"/>
+    <col min="6659" max="6659" width="20.5703125" customWidth="1"/>
     <col min="6660" max="6660" width="17" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6663" max="6663" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="21.453125" customWidth="1"/>
-    <col min="6914" max="6914" width="14.81640625" customWidth="1"/>
-    <col min="6915" max="6915" width="20.54296875" customWidth="1"/>
+    <col min="6661" max="6661" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="21.42578125" customWidth="1"/>
+    <col min="6914" max="6914" width="14.85546875" customWidth="1"/>
+    <col min="6915" max="6915" width="20.5703125" customWidth="1"/>
     <col min="6916" max="6916" width="17" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6919" max="6919" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="21.453125" customWidth="1"/>
-    <col min="7170" max="7170" width="14.81640625" customWidth="1"/>
-    <col min="7171" max="7171" width="20.54296875" customWidth="1"/>
+    <col min="6917" max="6917" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="21.42578125" customWidth="1"/>
+    <col min="7170" max="7170" width="14.85546875" customWidth="1"/>
+    <col min="7171" max="7171" width="20.5703125" customWidth="1"/>
     <col min="7172" max="7172" width="17" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7175" max="7175" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="21.453125" customWidth="1"/>
-    <col min="7426" max="7426" width="14.81640625" customWidth="1"/>
-    <col min="7427" max="7427" width="20.54296875" customWidth="1"/>
+    <col min="7173" max="7173" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="21.42578125" customWidth="1"/>
+    <col min="7426" max="7426" width="14.85546875" customWidth="1"/>
+    <col min="7427" max="7427" width="20.5703125" customWidth="1"/>
     <col min="7428" max="7428" width="17" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7431" max="7431" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="21.453125" customWidth="1"/>
-    <col min="7682" max="7682" width="14.81640625" customWidth="1"/>
-    <col min="7683" max="7683" width="20.54296875" customWidth="1"/>
+    <col min="7429" max="7429" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="21.42578125" customWidth="1"/>
+    <col min="7682" max="7682" width="14.85546875" customWidth="1"/>
+    <col min="7683" max="7683" width="20.5703125" customWidth="1"/>
     <col min="7684" max="7684" width="17" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7687" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="21.453125" customWidth="1"/>
-    <col min="7938" max="7938" width="14.81640625" customWidth="1"/>
-    <col min="7939" max="7939" width="20.54296875" customWidth="1"/>
+    <col min="7685" max="7685" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="21.42578125" customWidth="1"/>
+    <col min="7938" max="7938" width="14.85546875" customWidth="1"/>
+    <col min="7939" max="7939" width="20.5703125" customWidth="1"/>
     <col min="7940" max="7940" width="17" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7943" max="7943" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="21.453125" customWidth="1"/>
-    <col min="8194" max="8194" width="14.81640625" customWidth="1"/>
-    <col min="8195" max="8195" width="20.54296875" customWidth="1"/>
+    <col min="7941" max="7941" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="21.42578125" customWidth="1"/>
+    <col min="8194" max="8194" width="14.85546875" customWidth="1"/>
+    <col min="8195" max="8195" width="20.5703125" customWidth="1"/>
     <col min="8196" max="8196" width="17" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8199" max="8199" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="21.453125" customWidth="1"/>
-    <col min="8450" max="8450" width="14.81640625" customWidth="1"/>
-    <col min="8451" max="8451" width="20.54296875" customWidth="1"/>
+    <col min="8197" max="8197" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="21.42578125" customWidth="1"/>
+    <col min="8450" max="8450" width="14.85546875" customWidth="1"/>
+    <col min="8451" max="8451" width="20.5703125" customWidth="1"/>
     <col min="8452" max="8452" width="17" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8455" max="8455" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="21.453125" customWidth="1"/>
-    <col min="8706" max="8706" width="14.81640625" customWidth="1"/>
-    <col min="8707" max="8707" width="20.54296875" customWidth="1"/>
+    <col min="8453" max="8453" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="21.42578125" customWidth="1"/>
+    <col min="8706" max="8706" width="14.85546875" customWidth="1"/>
+    <col min="8707" max="8707" width="20.5703125" customWidth="1"/>
     <col min="8708" max="8708" width="17" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8711" max="8711" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="21.453125" customWidth="1"/>
-    <col min="8962" max="8962" width="14.81640625" customWidth="1"/>
-    <col min="8963" max="8963" width="20.54296875" customWidth="1"/>
+    <col min="8709" max="8709" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="21.42578125" customWidth="1"/>
+    <col min="8962" max="8962" width="14.85546875" customWidth="1"/>
+    <col min="8963" max="8963" width="20.5703125" customWidth="1"/>
     <col min="8964" max="8964" width="17" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8967" max="8967" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="21.453125" customWidth="1"/>
-    <col min="9218" max="9218" width="14.81640625" customWidth="1"/>
-    <col min="9219" max="9219" width="20.54296875" customWidth="1"/>
+    <col min="8965" max="8965" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="21.42578125" customWidth="1"/>
+    <col min="9218" max="9218" width="14.85546875" customWidth="1"/>
+    <col min="9219" max="9219" width="20.5703125" customWidth="1"/>
     <col min="9220" max="9220" width="17" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9223" max="9223" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="21.453125" customWidth="1"/>
-    <col min="9474" max="9474" width="14.81640625" customWidth="1"/>
-    <col min="9475" max="9475" width="20.54296875" customWidth="1"/>
+    <col min="9221" max="9221" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="21.42578125" customWidth="1"/>
+    <col min="9474" max="9474" width="14.85546875" customWidth="1"/>
+    <col min="9475" max="9475" width="20.5703125" customWidth="1"/>
     <col min="9476" max="9476" width="17" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9479" max="9479" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="21.453125" customWidth="1"/>
-    <col min="9730" max="9730" width="14.81640625" customWidth="1"/>
-    <col min="9731" max="9731" width="20.54296875" customWidth="1"/>
+    <col min="9477" max="9477" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="21.42578125" customWidth="1"/>
+    <col min="9730" max="9730" width="14.85546875" customWidth="1"/>
+    <col min="9731" max="9731" width="20.5703125" customWidth="1"/>
     <col min="9732" max="9732" width="17" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9735" max="9735" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="21.453125" customWidth="1"/>
-    <col min="9986" max="9986" width="14.81640625" customWidth="1"/>
-    <col min="9987" max="9987" width="20.54296875" customWidth="1"/>
+    <col min="9733" max="9733" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="21.42578125" customWidth="1"/>
+    <col min="9986" max="9986" width="14.85546875" customWidth="1"/>
+    <col min="9987" max="9987" width="20.5703125" customWidth="1"/>
     <col min="9988" max="9988" width="17" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9991" max="9991" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="21.453125" customWidth="1"/>
-    <col min="10242" max="10242" width="14.81640625" customWidth="1"/>
-    <col min="10243" max="10243" width="20.54296875" customWidth="1"/>
+    <col min="9989" max="9989" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="21.42578125" customWidth="1"/>
+    <col min="10242" max="10242" width="14.85546875" customWidth="1"/>
+    <col min="10243" max="10243" width="20.5703125" customWidth="1"/>
     <col min="10244" max="10244" width="17" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10247" max="10247" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="21.453125" customWidth="1"/>
-    <col min="10498" max="10498" width="14.81640625" customWidth="1"/>
-    <col min="10499" max="10499" width="20.54296875" customWidth="1"/>
+    <col min="10245" max="10245" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="21.42578125" customWidth="1"/>
+    <col min="10498" max="10498" width="14.85546875" customWidth="1"/>
+    <col min="10499" max="10499" width="20.5703125" customWidth="1"/>
     <col min="10500" max="10500" width="17" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10503" max="10503" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="21.453125" customWidth="1"/>
-    <col min="10754" max="10754" width="14.81640625" customWidth="1"/>
-    <col min="10755" max="10755" width="20.54296875" customWidth="1"/>
+    <col min="10501" max="10501" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="21.42578125" customWidth="1"/>
+    <col min="10754" max="10754" width="14.85546875" customWidth="1"/>
+    <col min="10755" max="10755" width="20.5703125" customWidth="1"/>
     <col min="10756" max="10756" width="17" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10759" max="10759" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="21.453125" customWidth="1"/>
-    <col min="11010" max="11010" width="14.81640625" customWidth="1"/>
-    <col min="11011" max="11011" width="20.54296875" customWidth="1"/>
+    <col min="10757" max="10757" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="21.42578125" customWidth="1"/>
+    <col min="11010" max="11010" width="14.85546875" customWidth="1"/>
+    <col min="11011" max="11011" width="20.5703125" customWidth="1"/>
     <col min="11012" max="11012" width="17" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11015" max="11015" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="21.453125" customWidth="1"/>
-    <col min="11266" max="11266" width="14.81640625" customWidth="1"/>
-    <col min="11267" max="11267" width="20.54296875" customWidth="1"/>
+    <col min="11013" max="11013" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="21.42578125" customWidth="1"/>
+    <col min="11266" max="11266" width="14.85546875" customWidth="1"/>
+    <col min="11267" max="11267" width="20.5703125" customWidth="1"/>
     <col min="11268" max="11268" width="17" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11271" max="11271" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="21.453125" customWidth="1"/>
-    <col min="11522" max="11522" width="14.81640625" customWidth="1"/>
-    <col min="11523" max="11523" width="20.54296875" customWidth="1"/>
+    <col min="11269" max="11269" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="21.42578125" customWidth="1"/>
+    <col min="11522" max="11522" width="14.85546875" customWidth="1"/>
+    <col min="11523" max="11523" width="20.5703125" customWidth="1"/>
     <col min="11524" max="11524" width="17" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11527" max="11527" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="21.453125" customWidth="1"/>
-    <col min="11778" max="11778" width="14.81640625" customWidth="1"/>
-    <col min="11779" max="11779" width="20.54296875" customWidth="1"/>
+    <col min="11525" max="11525" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="21.42578125" customWidth="1"/>
+    <col min="11778" max="11778" width="14.85546875" customWidth="1"/>
+    <col min="11779" max="11779" width="20.5703125" customWidth="1"/>
     <col min="11780" max="11780" width="17" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="11783" max="11783" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="21.453125" customWidth="1"/>
-    <col min="12034" max="12034" width="14.81640625" customWidth="1"/>
-    <col min="12035" max="12035" width="20.54296875" customWidth="1"/>
+    <col min="11781" max="11781" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="21.42578125" customWidth="1"/>
+    <col min="12034" max="12034" width="14.85546875" customWidth="1"/>
+    <col min="12035" max="12035" width="20.5703125" customWidth="1"/>
     <col min="12036" max="12036" width="17" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12039" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="21.453125" customWidth="1"/>
-    <col min="12290" max="12290" width="14.81640625" customWidth="1"/>
-    <col min="12291" max="12291" width="20.54296875" customWidth="1"/>
+    <col min="12037" max="12037" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="21.42578125" customWidth="1"/>
+    <col min="12290" max="12290" width="14.85546875" customWidth="1"/>
+    <col min="12291" max="12291" width="20.5703125" customWidth="1"/>
     <col min="12292" max="12292" width="17" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12295" max="12295" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="21.453125" customWidth="1"/>
-    <col min="12546" max="12546" width="14.81640625" customWidth="1"/>
-    <col min="12547" max="12547" width="20.54296875" customWidth="1"/>
+    <col min="12293" max="12293" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="21.42578125" customWidth="1"/>
+    <col min="12546" max="12546" width="14.85546875" customWidth="1"/>
+    <col min="12547" max="12547" width="20.5703125" customWidth="1"/>
     <col min="12548" max="12548" width="17" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12551" max="12551" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="21.453125" customWidth="1"/>
-    <col min="12802" max="12802" width="14.81640625" customWidth="1"/>
-    <col min="12803" max="12803" width="20.54296875" customWidth="1"/>
+    <col min="12549" max="12549" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="21.42578125" customWidth="1"/>
+    <col min="12802" max="12802" width="14.85546875" customWidth="1"/>
+    <col min="12803" max="12803" width="20.5703125" customWidth="1"/>
     <col min="12804" max="12804" width="17" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="12807" max="12807" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="21.453125" customWidth="1"/>
-    <col min="13058" max="13058" width="14.81640625" customWidth="1"/>
-    <col min="13059" max="13059" width="20.54296875" customWidth="1"/>
+    <col min="12805" max="12805" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="21.42578125" customWidth="1"/>
+    <col min="13058" max="13058" width="14.85546875" customWidth="1"/>
+    <col min="13059" max="13059" width="20.5703125" customWidth="1"/>
     <col min="13060" max="13060" width="17" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13063" max="13063" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="21.453125" customWidth="1"/>
-    <col min="13314" max="13314" width="14.81640625" customWidth="1"/>
-    <col min="13315" max="13315" width="20.54296875" customWidth="1"/>
+    <col min="13061" max="13061" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="21.42578125" customWidth="1"/>
+    <col min="13314" max="13314" width="14.85546875" customWidth="1"/>
+    <col min="13315" max="13315" width="20.5703125" customWidth="1"/>
     <col min="13316" max="13316" width="17" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13319" max="13319" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="21.453125" customWidth="1"/>
-    <col min="13570" max="13570" width="14.81640625" customWidth="1"/>
-    <col min="13571" max="13571" width="20.54296875" customWidth="1"/>
+    <col min="13317" max="13317" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="21.42578125" customWidth="1"/>
+    <col min="13570" max="13570" width="14.85546875" customWidth="1"/>
+    <col min="13571" max="13571" width="20.5703125" customWidth="1"/>
     <col min="13572" max="13572" width="17" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13575" max="13575" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="21.453125" customWidth="1"/>
-    <col min="13826" max="13826" width="14.81640625" customWidth="1"/>
-    <col min="13827" max="13827" width="20.54296875" customWidth="1"/>
+    <col min="13573" max="13573" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="21.42578125" customWidth="1"/>
+    <col min="13826" max="13826" width="14.85546875" customWidth="1"/>
+    <col min="13827" max="13827" width="20.5703125" customWidth="1"/>
     <col min="13828" max="13828" width="17" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13831" max="13831" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="21.453125" customWidth="1"/>
-    <col min="14082" max="14082" width="14.81640625" customWidth="1"/>
-    <col min="14083" max="14083" width="20.54296875" customWidth="1"/>
+    <col min="13829" max="13829" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="21.42578125" customWidth="1"/>
+    <col min="14082" max="14082" width="14.85546875" customWidth="1"/>
+    <col min="14083" max="14083" width="20.5703125" customWidth="1"/>
     <col min="14084" max="14084" width="17" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14087" max="14087" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="21.453125" customWidth="1"/>
-    <col min="14338" max="14338" width="14.81640625" customWidth="1"/>
-    <col min="14339" max="14339" width="20.54296875" customWidth="1"/>
+    <col min="14085" max="14085" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="21.42578125" customWidth="1"/>
+    <col min="14338" max="14338" width="14.85546875" customWidth="1"/>
+    <col min="14339" max="14339" width="20.5703125" customWidth="1"/>
     <col min="14340" max="14340" width="17" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14343" max="14343" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="21.453125" customWidth="1"/>
-    <col min="14594" max="14594" width="14.81640625" customWidth="1"/>
-    <col min="14595" max="14595" width="20.54296875" customWidth="1"/>
+    <col min="14341" max="14341" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="21.42578125" customWidth="1"/>
+    <col min="14594" max="14594" width="14.85546875" customWidth="1"/>
+    <col min="14595" max="14595" width="20.5703125" customWidth="1"/>
     <col min="14596" max="14596" width="17" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14599" max="14599" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="21.453125" customWidth="1"/>
-    <col min="14850" max="14850" width="14.81640625" customWidth="1"/>
-    <col min="14851" max="14851" width="20.54296875" customWidth="1"/>
+    <col min="14597" max="14597" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="21.42578125" customWidth="1"/>
+    <col min="14850" max="14850" width="14.85546875" customWidth="1"/>
+    <col min="14851" max="14851" width="20.5703125" customWidth="1"/>
     <col min="14852" max="14852" width="17" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="14855" max="14855" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="21.453125" customWidth="1"/>
-    <col min="15106" max="15106" width="14.81640625" customWidth="1"/>
-    <col min="15107" max="15107" width="20.54296875" customWidth="1"/>
+    <col min="14853" max="14853" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="21.42578125" customWidth="1"/>
+    <col min="15106" max="15106" width="14.85546875" customWidth="1"/>
+    <col min="15107" max="15107" width="20.5703125" customWidth="1"/>
     <col min="15108" max="15108" width="17" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15111" max="15111" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="21.453125" customWidth="1"/>
-    <col min="15362" max="15362" width="14.81640625" customWidth="1"/>
-    <col min="15363" max="15363" width="20.54296875" customWidth="1"/>
+    <col min="15109" max="15109" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="21.42578125" customWidth="1"/>
+    <col min="15362" max="15362" width="14.85546875" customWidth="1"/>
+    <col min="15363" max="15363" width="20.5703125" customWidth="1"/>
     <col min="15364" max="15364" width="17" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15367" max="15367" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="21.453125" customWidth="1"/>
-    <col min="15618" max="15618" width="14.81640625" customWidth="1"/>
-    <col min="15619" max="15619" width="20.54296875" customWidth="1"/>
+    <col min="15365" max="15365" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="21.42578125" customWidth="1"/>
+    <col min="15618" max="15618" width="14.85546875" customWidth="1"/>
+    <col min="15619" max="15619" width="20.5703125" customWidth="1"/>
     <col min="15620" max="15620" width="17" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15623" max="15623" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="21.453125" customWidth="1"/>
-    <col min="15874" max="15874" width="14.81640625" customWidth="1"/>
-    <col min="15875" max="15875" width="20.54296875" customWidth="1"/>
+    <col min="15621" max="15621" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="21.42578125" customWidth="1"/>
+    <col min="15874" max="15874" width="14.85546875" customWidth="1"/>
+    <col min="15875" max="15875" width="20.5703125" customWidth="1"/>
     <col min="15876" max="15876" width="17" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15879" max="15879" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="21.453125" customWidth="1"/>
-    <col min="16130" max="16130" width="14.81640625" customWidth="1"/>
-    <col min="16131" max="16131" width="20.54296875" customWidth="1"/>
+    <col min="15877" max="15877" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="21.42578125" customWidth="1"/>
+    <col min="16130" max="16130" width="14.85546875" customWidth="1"/>
+    <col min="16131" max="16131" width="20.5703125" customWidth="1"/>
     <col min="16132" max="16132" width="17" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="16135" max="16135" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -12133,7 +12522,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>887</v>
       </c>
@@ -12162,7 +12551,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1087</v>
       </c>
@@ -12191,7 +12580,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1087</v>
       </c>
@@ -12220,7 +12609,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1087</v>
       </c>
@@ -12249,7 +12638,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>887</v>
       </c>
@@ -12278,7 +12667,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>887</v>
       </c>
@@ -12307,7 +12696,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>887</v>
       </c>
@@ -12336,7 +12725,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>893</v>
       </c>
@@ -12365,7 +12754,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>910</v>
       </c>
@@ -12394,7 +12783,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>910</v>
       </c>
@@ -12423,7 +12812,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>893</v>
       </c>
@@ -12475,22 +12864,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12540,7 +12929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>562</v>
       </c>
@@ -12575,7 +12964,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>572</v>
       </c>
@@ -12610,7 +12999,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>659</v>
       </c>
@@ -12645,7 +13034,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>995</v>
       </c>
@@ -12680,7 +13069,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>740</v>
       </c>
@@ -12715,7 +13104,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>835</v>
       </c>
@@ -12748,7 +13137,7 @@
       </c>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>879</v>
       </c>
@@ -12783,7 +13172,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1028</v>
       </c>
@@ -12818,7 +13207,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>1040</v>
       </c>
@@ -12850,7 +13239,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1053</v>
       </c>
@@ -12899,9 +13288,9 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12964,28 +13353,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A03146-6FE6-45D1-B4C6-477159028F0E}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13038,7 +13427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -13076,7 +13465,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -13114,7 +13503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -13152,7 +13541,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>610</v>
       </c>
@@ -13190,7 +13579,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>717</v>
       </c>
@@ -13228,7 +13617,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>731</v>
       </c>
@@ -13266,7 +13655,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>746</v>
       </c>
@@ -13304,7 +13693,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>751</v>
       </c>
@@ -13342,7 +13731,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>755</v>
       </c>
@@ -13380,7 +13769,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>877</v>
       </c>
@@ -13418,7 +13807,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>885</v>
       </c>
@@ -13456,7 +13845,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>931</v>
       </c>
@@ -13494,7 +13883,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>973</v>
       </c>
@@ -13532,7 +13921,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>990</v>
       </c>
@@ -13567,7 +13956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1019</v>
       </c>
@@ -13605,7 +13994,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1073</v>
       </c>
@@ -13643,7 +14032,236 @@
         <v>1077</v>
       </c>
     </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>719</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>752</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>749</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19">
+        <v>1210</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>756</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>749</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20">
+        <v>1210</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>719</v>
+      </c>
+      <c r="I21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" t="s">
+        <v>719</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
+        <v>719</v>
+      </c>
+      <c r="I23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1149</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13656,22 +14274,22 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13724,7 +14342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>744272121</v>
       </c>
@@ -13759,7 +14377,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>635</v>
       </c>
@@ -13797,7 +14415,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>701</v>
       </c>
@@ -13832,7 +14450,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>759</v>
       </c>
@@ -13870,7 +14488,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1043</v>
       </c>
@@ -13908,7 +14526,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="28" ht="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" ht="13.35" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13923,9 +14541,9 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13945,7 +14563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>764</v>
       </c>
@@ -13978,18 +14596,18 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -14018,7 +14636,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>589</v>
       </c>
@@ -14047,7 +14665,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>589</v>
       </c>
@@ -14076,7 +14694,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>841</v>
       </c>
@@ -14121,21 +14739,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -14170,7 +14788,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>794</v>
       </c>
@@ -14205,7 +14823,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>790</v>
       </c>
@@ -14240,7 +14858,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>928</v>
       </c>
@@ -14292,21 +14910,21 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14353,7 +14971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>581</v>
       </c>
@@ -14385,7 +15003,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>603</v>
       </c>
@@ -14414,7 +15032,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>708</v>
       </c>
@@ -14446,7 +15064,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>828</v>
       </c>
@@ -14476,7 +15094,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>857</v>
       </c>
@@ -14505,7 +15123,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1007</v>
       </c>
@@ -14534,7 +15152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1012</v>
       </c>
@@ -14563,7 +15181,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1016</v>
       </c>
@@ -14586,7 +15204,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1083</v>
       </c>
@@ -14626,14 +15244,14 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14674,7 +15292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>648</v>
       </c>
@@ -14705,7 +15323,7 @@
       <c r="U2" s="7"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>649</v>
       </c>
@@ -14736,7 +15354,7 @@
       <c r="U3" s="7"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>650</v>
       </c>
@@ -14767,7 +15385,7 @@
       <c r="U4" s="7"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>651</v>
       </c>
@@ -14798,7 +15416,7 @@
       <c r="U5" s="7"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>652</v>
       </c>
@@ -14829,11 +15447,11 @@
       <c r="U6" s="7"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E7" s="7"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E8" s="7"/>
       <c r="H8" s="5"/>
     </row>
@@ -14847,24 +15465,25 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14911,7 +15530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>595</v>
       </c>
@@ -14943,7 +15562,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>666</v>
       </c>
@@ -14975,7 +15594,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>863</v>
       </c>
@@ -15007,7 +15626,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>958</v>
       </c>
@@ -15039,7 +15658,39 @@
         <v>961</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>582</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>668</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I9" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the L9963E footprint
Footprint was missing
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7873ED8-859B-4D11-A2BA-B2FFC9398771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123E11D-2C5C-42E0-8AFC-6D5A8D583422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -3244,9 +3244,6 @@
     <t>https://www.digikey.com.au/en/products/detail/te-connectivity-potter-brumfield-relays/1860991-1/11192373</t>
   </si>
   <si>
-    <t>ST_TQFP</t>
-  </si>
-  <si>
     <t>L9963E</t>
   </si>
   <si>
@@ -3701,6 +3698,9 @@
   </si>
   <si>
     <t>445-8637-1-ND</t>
+  </si>
+  <si>
+    <t>TQFP64_L9963E_STM</t>
   </si>
 </sst>
 </file>
@@ -10898,16 +10898,16 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B190" t="s">
         <v>1069</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="F190" t="s">
         <v>1071</v>
-      </c>
-      <c r="F190" t="s">
-        <v>1072</v>
       </c>
       <c r="G190" t="s">
         <v>722</v>
@@ -10924,10 +10924,10 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B191" t="s">
         <v>1078</v>
-      </c>
-      <c r="B191" t="s">
-        <v>1079</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>173</v>
@@ -10936,10 +10936,10 @@
         <v>0.01</v>
       </c>
       <c r="F191" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G191" t="s">
         <v>1080</v>
-      </c>
-      <c r="G191" t="s">
-        <v>1081</v>
       </c>
       <c r="H191" t="s">
         <v>33</v>
@@ -10951,15 +10951,15 @@
         <v>35</v>
       </c>
       <c r="M191" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B192" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>179</v>
@@ -10968,13 +10968,13 @@
         <v>0.01</v>
       </c>
       <c r="E192" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F192" t="s">
         <v>946</v>
       </c>
       <c r="G192" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H192" t="s">
         <v>33</v>
@@ -10986,50 +10986,50 @@
         <v>35</v>
       </c>
       <c r="M192" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B193" t="s">
         <v>1131</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="D193" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E193" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F193" t="s">
         <v>1133</v>
       </c>
-      <c r="D193" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E193" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F193" t="s">
+      <c r="G193" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H193" t="s">
+        <v>33</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="J193" t="s">
+        <v>35</v>
+      </c>
+      <c r="M193" t="s">
         <v>1134</v>
-      </c>
-      <c r="G193" t="s">
-        <v>1129</v>
-      </c>
-      <c r="H193" t="s">
-        <v>33</v>
-      </c>
-      <c r="I193" s="1" t="s">
-        <v>1130</v>
-      </c>
-      <c r="J193" t="s">
-        <v>35</v>
-      </c>
-      <c r="M193" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B194" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>945</v>
@@ -11038,7 +11038,7 @@
         <v>0.01</v>
       </c>
       <c r="E194" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F194">
         <v>0.5</v>
@@ -11056,15 +11056,15 @@
         <v>35</v>
       </c>
       <c r="M194" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B195" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>262</v>
@@ -11073,7 +11073,7 @@
         <v>0.01</v>
       </c>
       <c r="E195" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F195">
         <v>0.5</v>
@@ -11091,24 +11091,24 @@
         <v>35</v>
       </c>
       <c r="M195" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B196" t="s">
         <v>747</v>
       </c>
       <c r="C196" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F196" t="s">
         <v>1071</v>
       </c>
-      <c r="F196" t="s">
-        <v>1072</v>
-      </c>
       <c r="G196" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="H196" t="s">
         <v>33</v>
@@ -11120,12 +11120,12 @@
         <v>35</v>
       </c>
       <c r="M196" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B197" t="s">
         <v>55</v>
@@ -11155,18 +11155,18 @@
         <v>35</v>
       </c>
       <c r="M197" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B198" t="s">
+        <v>55</v>
+      </c>
+      <c r="C198" s="1" t="s">
         <v>1172</v>
-      </c>
-      <c r="B198" t="s">
-        <v>55</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>1173</v>
       </c>
       <c r="D198" s="2">
         <v>0.01</v>
@@ -11190,18 +11190,18 @@
         <v>35</v>
       </c>
       <c r="M198" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B199" t="s">
+        <v>55</v>
+      </c>
+      <c r="C199" s="1" t="s">
         <v>1175</v>
-      </c>
-      <c r="B199" t="s">
-        <v>55</v>
-      </c>
-      <c r="C199" s="1" t="s">
-        <v>1176</v>
       </c>
       <c r="D199" s="2">
         <v>0.01</v>
@@ -11225,7 +11225,7 @@
         <v>35</v>
       </c>
       <c r="M199" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -11240,8 +11240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12039,25 +12039,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D27" t="s">
         <v>1066</v>
       </c>
-      <c r="D27" t="s">
-        <v>1067</v>
-      </c>
       <c r="E27" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F27" t="s">
         <v>570</v>
       </c>
       <c r="G27" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="H27" t="s">
         <v>35</v>
@@ -12071,19 +12071,19 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D28" t="s">
         <v>1064</v>
       </c>
-      <c r="D28" t="s">
-        <v>1065</v>
-      </c>
       <c r="E28" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F28" t="s">
         <v>570</v>
       </c>
       <c r="G28" t="s">
-        <v>1063</v>
+        <v>1215</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -12091,34 +12091,34 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D29" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E29" t="s">
         <v>1100</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1101</v>
       </c>
       <c r="F29" t="s">
         <v>570</v>
       </c>
       <c r="G29" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J29" t="s">
         <v>1102</v>
-      </c>
-      <c r="H29" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" t="s">
-        <v>1104</v>
-      </c>
-      <c r="J29" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -12129,28 +12129,28 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D30" t="s">
         <v>1105</v>
       </c>
-      <c r="D30" t="s">
-        <v>1106</v>
-      </c>
       <c r="E30" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F30" t="s">
         <v>570</v>
       </c>
       <c r="G30" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="H30" t="s">
         <v>35</v>
       </c>
       <c r="I30" t="s">
+        <v>1106</v>
+      </c>
+      <c r="J30" t="s">
         <v>1107</v>
-      </c>
-      <c r="J30" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -12161,28 +12161,28 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D31" t="s">
         <v>1150</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>1151</v>
-      </c>
-      <c r="E31" t="s">
-        <v>1152</v>
       </c>
       <c r="F31" t="s">
         <v>570</v>
       </c>
       <c r="G31" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
         <v>1153</v>
       </c>
-      <c r="H31" t="s">
-        <v>35</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>1154</v>
-      </c>
-      <c r="J31" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -12193,28 +12193,28 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D32" t="s">
         <v>1156</v>
       </c>
-      <c r="D32" t="s">
-        <v>1157</v>
-      </c>
       <c r="E32" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F32" t="s">
         <v>570</v>
       </c>
       <c r="G32" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" t="s">
         <v>1158</v>
       </c>
-      <c r="H32" t="s">
-        <v>35</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>1159</v>
-      </c>
-      <c r="J32" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -12225,54 +12225,54 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D33" t="s">
         <v>1161</v>
       </c>
-      <c r="D33" t="s">
-        <v>1162</v>
-      </c>
       <c r="E33" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="F33" t="s">
         <v>570</v>
       </c>
       <c r="G33" t="s">
+        <v>1162</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
         <v>1163</v>
-      </c>
-      <c r="H33" t="s">
-        <v>35</v>
-      </c>
-      <c r="I33" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D34" t="s">
         <v>1166</v>
       </c>
-      <c r="D34" t="s">
-        <v>1167</v>
-      </c>
       <c r="E34" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F34" t="s">
         <v>570</v>
       </c>
       <c r="G34" t="s">
+        <v>1167</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" t="s">
         <v>1168</v>
-      </c>
-      <c r="H34" t="s">
-        <v>35</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1169</v>
       </c>
     </row>
   </sheetData>
@@ -12978,16 +12978,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C3" t="s">
         <v>1085</v>
       </c>
-      <c r="C3" t="s">
-        <v>1086</v>
-      </c>
       <c r="D3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E3" t="s">
         <v>570</v>
@@ -12999,24 +12999,24 @@
         <v>579</v>
       </c>
       <c r="H3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B4" t="s">
         <v>1087</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1088</v>
       </c>
-      <c r="C4" t="s">
-        <v>1089</v>
-      </c>
       <c r="D4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E4" t="s">
         <v>570</v>
@@ -13028,24 +13028,24 @@
         <v>579</v>
       </c>
       <c r="H4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D5" t="s">
         <v>1087</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1088</v>
       </c>
       <c r="E5" t="s">
         <v>570</v>
@@ -13057,10 +13057,10 @@
         <v>579</v>
       </c>
       <c r="H5" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -13701,89 +13701,89 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B12" t="s">
         <v>1183</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>1184</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>1185</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1186</v>
       </c>
       <c r="E12" t="s">
         <v>566</v>
       </c>
       <c r="F12" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G12" t="s">
         <v>1187</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1188</v>
       </c>
       <c r="H12" t="s">
         <v>570</v>
       </c>
       <c r="I12" t="s">
+        <v>1188</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" t="s">
         <v>1189</v>
-      </c>
-      <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" t="s">
-        <v>1190</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B13" t="s">
         <v>563</v>
       </c>
       <c r="C13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D13" t="s">
         <v>1192</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>1193</v>
       </c>
-      <c r="E13" t="s">
-        <v>1194</v>
-      </c>
       <c r="F13" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="G13" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H13" t="s">
         <v>570</v>
       </c>
       <c r="I13" t="s">
+        <v>1194</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" t="s">
         <v>1195</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1196</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B14" t="s">
         <v>563</v>
       </c>
       <c r="C14" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D14" t="s">
         <v>1198</v>
       </c>
-      <c r="D14" t="s">
-        <v>1199</v>
-      </c>
       <c r="E14" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="F14" t="s">
         <v>662</v>
@@ -13795,13 +13795,13 @@
         <v>570</v>
       </c>
       <c r="I14" t="s">
+        <v>1199</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" t="s">
         <v>1200</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1201</v>
       </c>
     </row>
   </sheetData>
@@ -14526,16 +14526,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B17" t="s">
         <v>747</v>
       </c>
       <c r="C17" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D17" t="s">
         <v>1074</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1075</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>47</v>
@@ -14544,7 +14544,7 @@
         <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="H17" t="s">
         <v>719</v>
@@ -14559,21 +14559,21 @@
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B18" t="s">
         <v>1110</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>1111</v>
       </c>
-      <c r="C18" t="s">
-        <v>1112</v>
-      </c>
       <c r="D18" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>47</v>
@@ -14597,21 +14597,21 @@
         <v>35</v>
       </c>
       <c r="N18" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B19" t="s">
         <v>1118</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1119</v>
       </c>
       <c r="C19" t="s">
         <v>752</v>
       </c>
       <c r="D19" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>47</v>
@@ -14635,21 +14635,21 @@
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B20" t="s">
         <v>1121</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1122</v>
       </c>
       <c r="C20" t="s">
         <v>756</v>
       </c>
       <c r="D20" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>47</v>
@@ -14673,21 +14673,21 @@
         <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C21" t="s">
         <v>1124</v>
       </c>
-      <c r="B21" t="s">
-        <v>1122</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1125</v>
-      </c>
       <c r="D21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>47</v>
@@ -14711,21 +14711,21 @@
         <v>35</v>
       </c>
       <c r="N21" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B22" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>47</v>
@@ -14749,21 +14749,21 @@
         <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B23" t="s">
         <v>1147</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1148</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>47</v>
@@ -14787,7 +14787,7 @@
         <v>35</v>
       </c>
       <c r="N23" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
   </sheetData>
@@ -14800,7 +14800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76B0024-F418-4661-B0F2-C53DE82765AF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -15058,7 +15058,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>999</v>
@@ -15070,10 +15070,10 @@
         <v>0.2</v>
       </c>
       <c r="E7" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F7" t="s">
         <v>1179</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1180</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>624</v>
@@ -15085,48 +15085,48 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
         <v>1181</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B8" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D8" s="2">
         <v>0.25</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>1211</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>1212</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>624</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>570</v>
       </c>
       <c r="J8" t="s">
+        <v>1213</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
         <v>1214</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="28" ht="13.35" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15328,13 +15328,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B5" t="s">
         <v>1202</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1204</v>
       </c>
       <c r="D5" t="s">
         <v>592</v>
@@ -15349,18 +15349,18 @@
         <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B6" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C6" t="s">
         <v>1206</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1207</v>
       </c>
       <c r="D6" t="s">
         <v>592</v>
@@ -15369,13 +15369,13 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
         <v>1208</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1209</v>
       </c>
     </row>
   </sheetData>
@@ -15861,13 +15861,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B10" t="s">
         <v>582</v>
       </c>
       <c r="D10" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E10" t="s">
         <v>584</v>
@@ -16315,34 +16315,34 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B6" t="s">
         <v>582</v>
       </c>
       <c r="C6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D6" t="s">
         <v>668</v>
       </c>
       <c r="E6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
         <v>1143</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1141</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1144</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MBED Added for TSAV Work
</commit_message>
<xml_diff>
--- a/components/ts_standard_library.xlsx
+++ b/components/ts_standard_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123E11D-2C5C-42E0-8AFC-6D5A8D583422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A5458F-49AD-46A4-AFBD-94FF5A485FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1545" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="1220">
   <si>
     <t>Part Number</t>
   </si>
@@ -3701,6 +3701,18 @@
   </si>
   <si>
     <t>TQFP64_L9963E_STM</t>
+  </si>
+  <si>
+    <t>MBED</t>
+  </si>
+  <si>
+    <t>Mbed Development Board LPC1768</t>
+  </si>
+  <si>
+    <t>LPC1768</t>
+  </si>
+  <si>
+    <t>LPC1768 MBED</t>
   </si>
 </sst>
 </file>
@@ -4088,19 +4100,19 @@
       <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4150,7 +4162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -4186,7 +4198,7 @@
       </c>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -4222,7 +4234,7 @@
       </c>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -4258,7 +4270,7 @@
       </c>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
@@ -4294,7 +4306,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -4330,7 +4342,7 @@
       </c>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -4366,7 +4378,7 @@
       </c>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -4402,7 +4414,7 @@
       </c>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
@@ -4438,7 +4450,7 @@
       </c>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -4474,7 +4486,7 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -4510,7 +4522,7 @@
       </c>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -4546,7 +4558,7 @@
       </c>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -4582,7 +4594,7 @@
       </c>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -4618,7 +4630,7 @@
       </c>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -4654,7 +4666,7 @@
       </c>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -4690,7 +4702,7 @@
       </c>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>103</v>
       </c>
@@ -4726,7 +4738,7 @@
       </c>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
@@ -4762,7 +4774,7 @@
       </c>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -4798,7 +4810,7 @@
       </c>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -4834,7 +4846,7 @@
       </c>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>115</v>
       </c>
@@ -4870,7 +4882,7 @@
       </c>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>118</v>
       </c>
@@ -4906,7 +4918,7 @@
       </c>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -4942,7 +4954,7 @@
       </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>124</v>
       </c>
@@ -4978,7 +4990,7 @@
       </c>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -5014,7 +5026,7 @@
       </c>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
@@ -5050,7 +5062,7 @@
       </c>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>133</v>
       </c>
@@ -5086,7 +5098,7 @@
       </c>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
@@ -5122,7 +5134,7 @@
       </c>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
@@ -5158,7 +5170,7 @@
       </c>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>142</v>
       </c>
@@ -5194,7 +5206,7 @@
       </c>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
@@ -5230,7 +5242,7 @@
       </c>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>148</v>
       </c>
@@ -5266,7 +5278,7 @@
       </c>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
@@ -5302,7 +5314,7 @@
       </c>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -5338,7 +5350,7 @@
       </c>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>157</v>
       </c>
@@ -5374,7 +5386,7 @@
       </c>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -5410,7 +5422,7 @@
       </c>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
@@ -5446,7 +5458,7 @@
       </c>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>166</v>
       </c>
@@ -5482,7 +5494,7 @@
       </c>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>169</v>
       </c>
@@ -5518,7 +5530,7 @@
       </c>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>172</v>
       </c>
@@ -5554,7 +5566,7 @@
       </c>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>175</v>
       </c>
@@ -5590,7 +5602,7 @@
       </c>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>178</v>
       </c>
@@ -5626,7 +5638,7 @@
       </c>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>181</v>
       </c>
@@ -5662,7 +5674,7 @@
       </c>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>184</v>
       </c>
@@ -5698,7 +5710,7 @@
       </c>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>187</v>
       </c>
@@ -5734,7 +5746,7 @@
       </c>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>190</v>
       </c>
@@ -5770,7 +5782,7 @@
       </c>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>193</v>
       </c>
@@ -5806,7 +5818,7 @@
       </c>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>196</v>
       </c>
@@ -5842,7 +5854,7 @@
       </c>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>199</v>
       </c>
@@ -5878,7 +5890,7 @@
       </c>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>202</v>
       </c>
@@ -5914,7 +5926,7 @@
       </c>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>205</v>
       </c>
@@ -5950,7 +5962,7 @@
       </c>
       <c r="T51" s="1"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>208</v>
       </c>
@@ -5986,7 +5998,7 @@
       </c>
       <c r="T52" s="1"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>211</v>
       </c>
@@ -6022,7 +6034,7 @@
       </c>
       <c r="T53" s="1"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>214</v>
       </c>
@@ -6058,7 +6070,7 @@
       </c>
       <c r="T54" s="1"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>217</v>
       </c>
@@ -6094,7 +6106,7 @@
       </c>
       <c r="T55" s="1"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>220</v>
       </c>
@@ -6130,7 +6142,7 @@
       </c>
       <c r="T56" s="1"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>223</v>
       </c>
@@ -6166,7 +6178,7 @@
       </c>
       <c r="T57" s="1"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -6202,7 +6214,7 @@
       </c>
       <c r="T58" s="1"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>228</v>
       </c>
@@ -6238,7 +6250,7 @@
       </c>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>231</v>
       </c>
@@ -6274,7 +6286,7 @@
       </c>
       <c r="T60" s="1"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
@@ -6310,7 +6322,7 @@
       </c>
       <c r="T61" s="1"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>237</v>
       </c>
@@ -6346,7 +6358,7 @@
       </c>
       <c r="T62" s="1"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>240</v>
       </c>
@@ -6382,7 +6394,7 @@
       </c>
       <c r="T63" s="1"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>243</v>
       </c>
@@ -6418,7 +6430,7 @@
       </c>
       <c r="T64" s="1"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>246</v>
       </c>
@@ -6454,7 +6466,7 @@
       </c>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>249</v>
       </c>
@@ -6490,7 +6502,7 @@
       </c>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>252</v>
       </c>
@@ -6526,7 +6538,7 @@
       </c>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>255</v>
       </c>
@@ -6562,7 +6574,7 @@
       </c>
       <c r="T68" s="1"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>258</v>
       </c>
@@ -6598,7 +6610,7 @@
       </c>
       <c r="T69" s="1"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>261</v>
       </c>
@@ -6634,7 +6646,7 @@
       </c>
       <c r="T70" s="1"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>264</v>
       </c>
@@ -6670,7 +6682,7 @@
       </c>
       <c r="T71" s="1"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>267</v>
       </c>
@@ -6706,7 +6718,7 @@
       </c>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>270</v>
       </c>
@@ -6742,7 +6754,7 @@
       </c>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>273</v>
       </c>
@@ -6778,7 +6790,7 @@
       </c>
       <c r="T74" s="1"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>276</v>
       </c>
@@ -6814,7 +6826,7 @@
       </c>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>279</v>
       </c>
@@ -6850,7 +6862,7 @@
       </c>
       <c r="T76" s="1"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6886,7 +6898,7 @@
       </c>
       <c r="T77" s="1"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6922,7 +6934,7 @@
       </c>
       <c r="T78" s="1"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>288</v>
       </c>
@@ -6958,7 +6970,7 @@
       </c>
       <c r="T79" s="1"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>291</v>
       </c>
@@ -6994,7 +7006,7 @@
       </c>
       <c r="T80" s="1"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>294</v>
       </c>
@@ -7030,7 +7042,7 @@
       </c>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>297</v>
       </c>
@@ -7066,7 +7078,7 @@
       </c>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>300</v>
       </c>
@@ -7102,7 +7114,7 @@
       </c>
       <c r="T83" s="1"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>303</v>
       </c>
@@ -7138,7 +7150,7 @@
       </c>
       <c r="T84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>306</v>
       </c>
@@ -7174,7 +7186,7 @@
       </c>
       <c r="T85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>309</v>
       </c>
@@ -7210,7 +7222,7 @@
       </c>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>312</v>
       </c>
@@ -7246,7 +7258,7 @@
       </c>
       <c r="T87" s="1"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>315</v>
       </c>
@@ -7282,7 +7294,7 @@
       </c>
       <c r="T88" s="1"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>318</v>
       </c>
@@ -7318,7 +7330,7 @@
       </c>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>321</v>
       </c>
@@ -7354,7 +7366,7 @@
       </c>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>324</v>
       </c>
@@ -7390,7 +7402,7 @@
       </c>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>327</v>
       </c>
@@ -7426,7 +7438,7 @@
       </c>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>330</v>
       </c>
@@ -7462,7 +7474,7 @@
       </c>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>333</v>
       </c>
@@ -7498,7 +7510,7 @@
       </c>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>336</v>
       </c>
@@ -7534,7 +7546,7 @@
       </c>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>339</v>
       </c>
@@ -7570,7 +7582,7 @@
       </c>
       <c r="T96" s="1"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>342</v>
       </c>
@@ -7606,7 +7618,7 @@
       </c>
       <c r="T97" s="1"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>345</v>
       </c>
@@ -7642,7 +7654,7 @@
       </c>
       <c r="T98" s="1"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>348</v>
       </c>
@@ -7678,7 +7690,7 @@
       </c>
       <c r="T99" s="1"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>351</v>
       </c>
@@ -7714,7 +7726,7 @@
       </c>
       <c r="T100" s="1"/>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>354</v>
       </c>
@@ -7750,7 +7762,7 @@
       </c>
       <c r="T101" s="1"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>357</v>
       </c>
@@ -7786,7 +7798,7 @@
       </c>
       <c r="T102" s="1"/>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>360</v>
       </c>
@@ -7822,7 +7834,7 @@
       </c>
       <c r="T103" s="1"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>363</v>
       </c>
@@ -7858,7 +7870,7 @@
       </c>
       <c r="T104" s="1"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>366</v>
       </c>
@@ -7894,7 +7906,7 @@
       </c>
       <c r="T105" s="1"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>369</v>
       </c>
@@ -7930,7 +7942,7 @@
       </c>
       <c r="T106" s="1"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>372</v>
       </c>
@@ -7966,7 +7978,7 @@
       </c>
       <c r="T107" s="1"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>375</v>
       </c>
@@ -8002,7 +8014,7 @@
       </c>
       <c r="T108" s="1"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>378</v>
       </c>
@@ -8038,7 +8050,7 @@
       </c>
       <c r="T109" s="1"/>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>381</v>
       </c>
@@ -8074,7 +8086,7 @@
       </c>
       <c r="T110" s="1"/>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>384</v>
       </c>
@@ -8110,7 +8122,7 @@
       </c>
       <c r="T111" s="1"/>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>387</v>
       </c>
@@ -8146,7 +8158,7 @@
       </c>
       <c r="T112" s="1"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>390</v>
       </c>
@@ -8182,7 +8194,7 @@
       </c>
       <c r="T113" s="1"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>393</v>
       </c>
@@ -8218,7 +8230,7 @@
       </c>
       <c r="T114" s="1"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>396</v>
       </c>
@@ -8254,7 +8266,7 @@
       </c>
       <c r="T115" s="1"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>399</v>
       </c>
@@ -8290,7 +8302,7 @@
       </c>
       <c r="T116" s="1"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>402</v>
       </c>
@@ -8326,7 +8338,7 @@
       </c>
       <c r="T117" s="1"/>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>402</v>
       </c>
@@ -8362,7 +8374,7 @@
       </c>
       <c r="T118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>407</v>
       </c>
@@ -8398,7 +8410,7 @@
       </c>
       <c r="T119" s="1"/>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>410</v>
       </c>
@@ -8434,7 +8446,7 @@
       </c>
       <c r="T120" s="1"/>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>413</v>
       </c>
@@ -8470,7 +8482,7 @@
       </c>
       <c r="T121" s="1"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>416</v>
       </c>
@@ -8507,7 +8519,7 @@
       </c>
       <c r="T122" s="1"/>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>419</v>
       </c>
@@ -8544,7 +8556,7 @@
       </c>
       <c r="T123" s="1"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>422</v>
       </c>
@@ -8581,7 +8593,7 @@
       </c>
       <c r="T124" s="1"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>424</v>
       </c>
@@ -8618,7 +8630,7 @@
       </c>
       <c r="T125" s="1"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>427</v>
       </c>
@@ -8655,7 +8667,7 @@
       </c>
       <c r="T126" s="1"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>430</v>
       </c>
@@ -8692,7 +8704,7 @@
       </c>
       <c r="T127" s="1"/>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>433</v>
       </c>
@@ -8729,7 +8741,7 @@
       </c>
       <c r="T128" s="1"/>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>436</v>
       </c>
@@ -8766,7 +8778,7 @@
       </c>
       <c r="T129" s="1"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>439</v>
       </c>
@@ -8803,7 +8815,7 @@
       </c>
       <c r="T130" s="1"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>442</v>
       </c>
@@ -8840,7 +8852,7 @@
       </c>
       <c r="T131" s="1"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>445</v>
       </c>
@@ -8877,7 +8889,7 @@
       </c>
       <c r="T132" s="1"/>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>448</v>
       </c>
@@ -8914,7 +8926,7 @@
       </c>
       <c r="T133" s="1"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>451</v>
       </c>
@@ -8951,7 +8963,7 @@
       </c>
       <c r="T134" s="1"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>454</v>
       </c>
@@ -8988,7 +9000,7 @@
       </c>
       <c r="T135" s="1"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>457</v>
       </c>
@@ -9025,7 +9037,7 @@
       </c>
       <c r="T136" s="1"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>460</v>
       </c>
@@ -9062,7 +9074,7 @@
       </c>
       <c r="T137" s="1"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>463</v>
       </c>
@@ -9099,7 +9111,7 @@
       </c>
       <c r="T138" s="1"/>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>466</v>
       </c>
@@ -9136,7 +9148,7 @@
       </c>
       <c r="T139" s="1"/>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>469</v>
       </c>
@@ -9173,7 +9185,7 @@
       </c>
       <c r="T140" s="1"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>472</v>
       </c>
@@ -9210,7 +9222,7 @@
       </c>
       <c r="T141" s="1"/>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>475</v>
       </c>
@@ -9247,7 +9259,7 @@
       </c>
       <c r="T142" s="1"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>478</v>
       </c>
@@ -9284,7 +9296,7 @@
       </c>
       <c r="T143" s="1"/>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>481</v>
       </c>
@@ -9321,7 +9333,7 @@
       </c>
       <c r="T144" s="1"/>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>484</v>
       </c>
@@ -9358,7 +9370,7 @@
       </c>
       <c r="T145" s="1"/>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>487</v>
       </c>
@@ -9394,7 +9406,7 @@
       </c>
       <c r="T146" s="1"/>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>490</v>
       </c>
@@ -9430,7 +9442,7 @@
       </c>
       <c r="T147" s="1"/>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>493</v>
       </c>
@@ -9466,7 +9478,7 @@
       </c>
       <c r="T148" s="1"/>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>496</v>
       </c>
@@ -9502,7 +9514,7 @@
       </c>
       <c r="T149" s="1"/>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>499</v>
       </c>
@@ -9538,7 +9550,7 @@
       </c>
       <c r="T150" s="1"/>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>502</v>
       </c>
@@ -9574,7 +9586,7 @@
       </c>
       <c r="T151" s="1"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>505</v>
       </c>
@@ -9610,7 +9622,7 @@
       </c>
       <c r="T152" s="1"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>508</v>
       </c>
@@ -9646,7 +9658,7 @@
       </c>
       <c r="T153" s="1"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>511</v>
       </c>
@@ -9682,7 +9694,7 @@
       </c>
       <c r="T154" s="1"/>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>514</v>
       </c>
@@ -9718,7 +9730,7 @@
       </c>
       <c r="T155" s="1"/>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>517</v>
       </c>
@@ -9754,7 +9766,7 @@
       </c>
       <c r="T156" s="1"/>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>520</v>
       </c>
@@ -9790,7 +9802,7 @@
       </c>
       <c r="T157" s="1"/>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>523</v>
       </c>
@@ -9826,7 +9838,7 @@
       </c>
       <c r="T158" s="1"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>526</v>
       </c>
@@ -9862,7 +9874,7 @@
       </c>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>529</v>
       </c>
@@ -9898,7 +9910,7 @@
       </c>
       <c r="T160" s="1"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>532</v>
       </c>
@@ -9934,7 +9946,7 @@
       </c>
       <c r="T161" s="1"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>535</v>
       </c>
@@ -9970,7 +9982,7 @@
       </c>
       <c r="T162" s="1"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>538</v>
       </c>
@@ -10006,7 +10018,7 @@
       </c>
       <c r="T163" s="1"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>541</v>
       </c>
@@ -10042,7 +10054,7 @@
       </c>
       <c r="T164" s="1"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>544</v>
       </c>
@@ -10078,7 +10090,7 @@
       </c>
       <c r="T165" s="1"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>547</v>
       </c>
@@ -10114,7 +10126,7 @@
       </c>
       <c r="T166" s="1"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>550</v>
       </c>
@@ -10150,7 +10162,7 @@
       </c>
       <c r="T167" s="1"/>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>553</v>
       </c>
@@ -10186,7 +10198,7 @@
       </c>
       <c r="T168" s="1"/>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>556</v>
       </c>
@@ -10222,7 +10234,7 @@
       </c>
       <c r="T169" s="1"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>559</v>
       </c>
@@ -10258,7 +10270,7 @@
       </c>
       <c r="T170" s="1"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>678</v>
       </c>
@@ -10290,7 +10302,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>733</v>
       </c>
@@ -10325,7 +10337,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>723</v>
       </c>
@@ -10360,7 +10372,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>735</v>
       </c>
@@ -10395,7 +10407,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>730</v>
       </c>
@@ -10430,7 +10442,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>851</v>
       </c>
@@ -10462,7 +10474,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>873</v>
       </c>
@@ -10497,7 +10509,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>929</v>
       </c>
@@ -10532,7 +10544,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>933</v>
       </c>
@@ -10567,7 +10579,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>936</v>
       </c>
@@ -10602,7 +10614,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>942</v>
       </c>
@@ -10634,7 +10646,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>943</v>
       </c>
@@ -10666,7 +10678,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>956</v>
       </c>
@@ -10701,7 +10713,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>969</v>
       </c>
@@ -10736,7 +10748,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>971</v>
       </c>
@@ -10771,7 +10783,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>1002</v>
       </c>
@@ -10803,7 +10815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>1022</v>
       </c>
@@ -10835,7 +10847,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>1039</v>
       </c>
@@ -10864,7 +10876,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>1049</v>
       </c>
@@ -10896,7 +10908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>1068</v>
       </c>
@@ -10922,7 +10934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>1077</v>
       </c>
@@ -10954,7 +10966,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>1113</v>
       </c>
@@ -10989,7 +11001,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>1130</v>
       </c>
@@ -11024,7 +11036,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>1135</v>
       </c>
@@ -11059,7 +11071,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>1137</v>
       </c>
@@ -11094,7 +11106,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>1144</v>
       </c>
@@ -11123,7 +11135,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>1169</v>
       </c>
@@ -11158,7 +11170,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>1171</v>
       </c>
@@ -11193,7 +11205,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>1174</v>
       </c>
@@ -11238,27 +11250,27 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1DE6D1-9EC9-4629-A776-8010F0778D63}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="98.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
+    <col min="9" max="9" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="148" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11291,7 +11303,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>582</v>
       </c>
@@ -11323,7 +11335,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>689</v>
       </c>
@@ -11355,7 +11367,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>695</v>
       </c>
@@ -11387,7 +11399,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>774</v>
       </c>
@@ -11419,7 +11431,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>780</v>
       </c>
@@ -11451,7 +11463,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>582</v>
       </c>
@@ -11483,7 +11495,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>774</v>
       </c>
@@ -11515,7 +11527,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>737</v>
       </c>
@@ -11547,7 +11559,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>774</v>
       </c>
@@ -11579,7 +11591,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>737</v>
       </c>
@@ -11611,7 +11623,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>563</v>
       </c>
@@ -11643,7 +11655,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>924</v>
       </c>
@@ -11675,7 +11687,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>563</v>
       </c>
@@ -11701,7 +11713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>563</v>
       </c>
@@ -11730,7 +11742,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>689</v>
       </c>
@@ -11762,7 +11774,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>689</v>
       </c>
@@ -11788,7 +11800,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>563</v>
       </c>
@@ -11817,7 +11829,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>563</v>
       </c>
@@ -11849,7 +11861,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>737</v>
       </c>
@@ -11875,7 +11887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>689</v>
       </c>
@@ -11901,7 +11913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>689</v>
       </c>
@@ -11927,7 +11939,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>689</v>
       </c>
@@ -11953,7 +11965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>563</v>
       </c>
@@ -11985,7 +11997,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>563</v>
       </c>
@@ -12011,7 +12023,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>563</v>
       </c>
@@ -12037,7 +12049,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1067</v>
       </c>
@@ -12063,7 +12075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>924</v>
       </c>
@@ -12089,7 +12101,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1098</v>
       </c>
@@ -12121,7 +12133,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>582</v>
       </c>
@@ -12153,7 +12165,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>563</v>
       </c>
@@ -12185,7 +12197,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>563</v>
       </c>
@@ -12217,7 +12229,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>563</v>
       </c>
@@ -12246,7 +12258,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1164</v>
       </c>
@@ -12273,6 +12285,32 @@
       </c>
       <c r="I34" t="s">
         <v>1168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F35" t="s">
+        <v>570</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H35" t="s">
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -12299,18 +12337,18 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12357,7 +12395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>672</v>
       </c>
@@ -12402,523 +12440,523 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="21.42578125" customWidth="1"/>
-    <col min="258" max="258" width="14.85546875" customWidth="1"/>
-    <col min="259" max="259" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="21.453125" customWidth="1"/>
+    <col min="258" max="258" width="14.81640625" customWidth="1"/>
+    <col min="259" max="259" width="20.54296875" customWidth="1"/>
     <col min="260" max="260" width="17" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="21.42578125" customWidth="1"/>
-    <col min="514" max="514" width="14.85546875" customWidth="1"/>
-    <col min="515" max="515" width="20.5703125" customWidth="1"/>
+    <col min="261" max="261" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="21.453125" customWidth="1"/>
+    <col min="514" max="514" width="14.81640625" customWidth="1"/>
+    <col min="515" max="515" width="20.54296875" customWidth="1"/>
     <col min="516" max="516" width="17" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="21.42578125" customWidth="1"/>
-    <col min="770" max="770" width="14.85546875" customWidth="1"/>
-    <col min="771" max="771" width="20.5703125" customWidth="1"/>
+    <col min="517" max="517" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="21.453125" customWidth="1"/>
+    <col min="770" max="770" width="14.81640625" customWidth="1"/>
+    <col min="771" max="771" width="20.54296875" customWidth="1"/>
     <col min="772" max="772" width="17" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="775" max="775" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="21.42578125" customWidth="1"/>
-    <col min="1026" max="1026" width="14.85546875" customWidth="1"/>
-    <col min="1027" max="1027" width="20.5703125" customWidth="1"/>
+    <col min="773" max="773" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="21.453125" customWidth="1"/>
+    <col min="1026" max="1026" width="14.81640625" customWidth="1"/>
+    <col min="1027" max="1027" width="20.54296875" customWidth="1"/>
     <col min="1028" max="1028" width="17" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="1031" max="1031" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="21.42578125" customWidth="1"/>
-    <col min="1282" max="1282" width="14.85546875" customWidth="1"/>
-    <col min="1283" max="1283" width="20.5703125" customWidth="1"/>
+    <col min="1029" max="1029" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="21.453125" customWidth="1"/>
+    <col min="1282" max="1282" width="14.81640625" customWidth="1"/>
+    <col min="1283" max="1283" width="20.54296875" customWidth="1"/>
     <col min="1284" max="1284" width="17" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="1287" max="1287" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="21.42578125" customWidth="1"/>
-    <col min="1538" max="1538" width="14.85546875" customWidth="1"/>
-    <col min="1539" max="1539" width="20.5703125" customWidth="1"/>
+    <col min="1285" max="1285" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="21.453125" customWidth="1"/>
+    <col min="1538" max="1538" width="14.81640625" customWidth="1"/>
+    <col min="1539" max="1539" width="20.54296875" customWidth="1"/>
     <col min="1540" max="1540" width="17" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="1543" max="1543" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="21.42578125" customWidth="1"/>
-    <col min="1794" max="1794" width="14.85546875" customWidth="1"/>
-    <col min="1795" max="1795" width="20.5703125" customWidth="1"/>
+    <col min="1541" max="1541" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="21.453125" customWidth="1"/>
+    <col min="1794" max="1794" width="14.81640625" customWidth="1"/>
+    <col min="1795" max="1795" width="20.54296875" customWidth="1"/>
     <col min="1796" max="1796" width="17" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="1799" max="1799" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="21.42578125" customWidth="1"/>
-    <col min="2050" max="2050" width="14.85546875" customWidth="1"/>
-    <col min="2051" max="2051" width="20.5703125" customWidth="1"/>
+    <col min="1797" max="1797" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="21.453125" customWidth="1"/>
+    <col min="2050" max="2050" width="14.81640625" customWidth="1"/>
+    <col min="2051" max="2051" width="20.54296875" customWidth="1"/>
     <col min="2052" max="2052" width="17" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2055" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="21.42578125" customWidth="1"/>
-    <col min="2306" max="2306" width="14.85546875" customWidth="1"/>
-    <col min="2307" max="2307" width="20.5703125" customWidth="1"/>
+    <col min="2053" max="2053" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="21.453125" customWidth="1"/>
+    <col min="2306" max="2306" width="14.81640625" customWidth="1"/>
+    <col min="2307" max="2307" width="20.54296875" customWidth="1"/>
     <col min="2308" max="2308" width="17" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2311" max="2311" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="21.42578125" customWidth="1"/>
-    <col min="2562" max="2562" width="14.85546875" customWidth="1"/>
-    <col min="2563" max="2563" width="20.5703125" customWidth="1"/>
+    <col min="2309" max="2309" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="21.453125" customWidth="1"/>
+    <col min="2562" max="2562" width="14.81640625" customWidth="1"/>
+    <col min="2563" max="2563" width="20.54296875" customWidth="1"/>
     <col min="2564" max="2564" width="17" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2567" max="2567" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="21.42578125" customWidth="1"/>
-    <col min="2818" max="2818" width="14.85546875" customWidth="1"/>
-    <col min="2819" max="2819" width="20.5703125" customWidth="1"/>
+    <col min="2565" max="2565" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="21.453125" customWidth="1"/>
+    <col min="2818" max="2818" width="14.81640625" customWidth="1"/>
+    <col min="2819" max="2819" width="20.54296875" customWidth="1"/>
     <col min="2820" max="2820" width="17" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2823" max="2823" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="21.42578125" customWidth="1"/>
-    <col min="3074" max="3074" width="14.85546875" customWidth="1"/>
-    <col min="3075" max="3075" width="20.5703125" customWidth="1"/>
+    <col min="2821" max="2821" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="21.453125" customWidth="1"/>
+    <col min="3074" max="3074" width="14.81640625" customWidth="1"/>
+    <col min="3075" max="3075" width="20.54296875" customWidth="1"/>
     <col min="3076" max="3076" width="17" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3079" max="3079" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="21.42578125" customWidth="1"/>
-    <col min="3330" max="3330" width="14.85546875" customWidth="1"/>
-    <col min="3331" max="3331" width="20.5703125" customWidth="1"/>
+    <col min="3077" max="3077" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="21.453125" customWidth="1"/>
+    <col min="3330" max="3330" width="14.81640625" customWidth="1"/>
+    <col min="3331" max="3331" width="20.54296875" customWidth="1"/>
     <col min="3332" max="3332" width="17" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3335" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="21.42578125" customWidth="1"/>
-    <col min="3586" max="3586" width="14.85546875" customWidth="1"/>
-    <col min="3587" max="3587" width="20.5703125" customWidth="1"/>
+    <col min="3333" max="3333" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="21.453125" customWidth="1"/>
+    <col min="3586" max="3586" width="14.81640625" customWidth="1"/>
+    <col min="3587" max="3587" width="20.54296875" customWidth="1"/>
     <col min="3588" max="3588" width="17" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3591" max="3591" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="21.42578125" customWidth="1"/>
-    <col min="3842" max="3842" width="14.85546875" customWidth="1"/>
-    <col min="3843" max="3843" width="20.5703125" customWidth="1"/>
+    <col min="3589" max="3589" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="21.453125" customWidth="1"/>
+    <col min="3842" max="3842" width="14.81640625" customWidth="1"/>
+    <col min="3843" max="3843" width="20.54296875" customWidth="1"/>
     <col min="3844" max="3844" width="17" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3847" max="3847" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="21.42578125" customWidth="1"/>
-    <col min="4098" max="4098" width="14.85546875" customWidth="1"/>
-    <col min="4099" max="4099" width="20.5703125" customWidth="1"/>
+    <col min="3845" max="3845" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="21.453125" customWidth="1"/>
+    <col min="4098" max="4098" width="14.81640625" customWidth="1"/>
+    <col min="4099" max="4099" width="20.54296875" customWidth="1"/>
     <col min="4100" max="4100" width="17" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4103" max="4103" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="21.42578125" customWidth="1"/>
-    <col min="4354" max="4354" width="14.85546875" customWidth="1"/>
-    <col min="4355" max="4355" width="20.5703125" customWidth="1"/>
+    <col min="4101" max="4101" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="21.453125" customWidth="1"/>
+    <col min="4354" max="4354" width="14.81640625" customWidth="1"/>
+    <col min="4355" max="4355" width="20.54296875" customWidth="1"/>
     <col min="4356" max="4356" width="17" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4359" max="4359" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="21.42578125" customWidth="1"/>
-    <col min="4610" max="4610" width="14.85546875" customWidth="1"/>
-    <col min="4611" max="4611" width="20.5703125" customWidth="1"/>
+    <col min="4357" max="4357" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="21.453125" customWidth="1"/>
+    <col min="4610" max="4610" width="14.81640625" customWidth="1"/>
+    <col min="4611" max="4611" width="20.54296875" customWidth="1"/>
     <col min="4612" max="4612" width="17" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4615" max="4615" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="21.42578125" customWidth="1"/>
-    <col min="4866" max="4866" width="14.85546875" customWidth="1"/>
-    <col min="4867" max="4867" width="20.5703125" customWidth="1"/>
+    <col min="4613" max="4613" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="21.453125" customWidth="1"/>
+    <col min="4866" max="4866" width="14.81640625" customWidth="1"/>
+    <col min="4867" max="4867" width="20.54296875" customWidth="1"/>
     <col min="4868" max="4868" width="17" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4871" max="4871" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="21.42578125" customWidth="1"/>
-    <col min="5122" max="5122" width="14.85546875" customWidth="1"/>
-    <col min="5123" max="5123" width="20.5703125" customWidth="1"/>
+    <col min="4869" max="4869" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="21.453125" customWidth="1"/>
+    <col min="5122" max="5122" width="14.81640625" customWidth="1"/>
+    <col min="5123" max="5123" width="20.54296875" customWidth="1"/>
     <col min="5124" max="5124" width="17" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5127" max="5127" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="21.42578125" customWidth="1"/>
-    <col min="5378" max="5378" width="14.85546875" customWidth="1"/>
-    <col min="5379" max="5379" width="20.5703125" customWidth="1"/>
+    <col min="5125" max="5125" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="21.453125" customWidth="1"/>
+    <col min="5378" max="5378" width="14.81640625" customWidth="1"/>
+    <col min="5379" max="5379" width="20.54296875" customWidth="1"/>
     <col min="5380" max="5380" width="17" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5383" max="5383" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="21.42578125" customWidth="1"/>
-    <col min="5634" max="5634" width="14.85546875" customWidth="1"/>
-    <col min="5635" max="5635" width="20.5703125" customWidth="1"/>
+    <col min="5381" max="5381" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="21.453125" customWidth="1"/>
+    <col min="5634" max="5634" width="14.81640625" customWidth="1"/>
+    <col min="5635" max="5635" width="20.54296875" customWidth="1"/>
     <col min="5636" max="5636" width="17" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5639" max="5639" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="21.42578125" customWidth="1"/>
-    <col min="5890" max="5890" width="14.85546875" customWidth="1"/>
-    <col min="5891" max="5891" width="20.5703125" customWidth="1"/>
+    <col min="5637" max="5637" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="21.453125" customWidth="1"/>
+    <col min="5890" max="5890" width="14.81640625" customWidth="1"/>
+    <col min="5891" max="5891" width="20.54296875" customWidth="1"/>
     <col min="5892" max="5892" width="17" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5895" max="5895" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="21.42578125" customWidth="1"/>
-    <col min="6146" max="6146" width="14.85546875" customWidth="1"/>
-    <col min="6147" max="6147" width="20.5703125" customWidth="1"/>
+    <col min="5893" max="5893" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="21.453125" customWidth="1"/>
+    <col min="6146" max="6146" width="14.81640625" customWidth="1"/>
+    <col min="6147" max="6147" width="20.54296875" customWidth="1"/>
     <col min="6148" max="6148" width="17" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6151" max="6151" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="21.42578125" customWidth="1"/>
-    <col min="6402" max="6402" width="14.85546875" customWidth="1"/>
-    <col min="6403" max="6403" width="20.5703125" customWidth="1"/>
+    <col min="6149" max="6149" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="21.453125" customWidth="1"/>
+    <col min="6402" max="6402" width="14.81640625" customWidth="1"/>
+    <col min="6403" max="6403" width="20.54296875" customWidth="1"/>
     <col min="6404" max="6404" width="17" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6407" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="21.42578125" customWidth="1"/>
-    <col min="6658" max="6658" width="14.85546875" customWidth="1"/>
-    <col min="6659" max="6659" width="20.5703125" customWidth="1"/>
+    <col min="6405" max="6405" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="21.453125" customWidth="1"/>
+    <col min="6658" max="6658" width="14.81640625" customWidth="1"/>
+    <col min="6659" max="6659" width="20.54296875" customWidth="1"/>
     <col min="6660" max="6660" width="17" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6663" max="6663" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="21.42578125" customWidth="1"/>
-    <col min="6914" max="6914" width="14.85546875" customWidth="1"/>
-    <col min="6915" max="6915" width="20.5703125" customWidth="1"/>
+    <col min="6661" max="6661" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="21.453125" customWidth="1"/>
+    <col min="6914" max="6914" width="14.81640625" customWidth="1"/>
+    <col min="6915" max="6915" width="20.54296875" customWidth="1"/>
     <col min="6916" max="6916" width="17" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6919" max="6919" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="21.42578125" customWidth="1"/>
-    <col min="7170" max="7170" width="14.85546875" customWidth="1"/>
-    <col min="7171" max="7171" width="20.5703125" customWidth="1"/>
+    <col min="6917" max="6917" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="21.453125" customWidth="1"/>
+    <col min="7170" max="7170" width="14.81640625" customWidth="1"/>
+    <col min="7171" max="7171" width="20.54296875" customWidth="1"/>
     <col min="7172" max="7172" width="17" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7175" max="7175" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="21.42578125" customWidth="1"/>
-    <col min="7426" max="7426" width="14.85546875" customWidth="1"/>
-    <col min="7427" max="7427" width="20.5703125" customWidth="1"/>
+    <col min="7173" max="7173" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="21.453125" customWidth="1"/>
+    <col min="7426" max="7426" width="14.81640625" customWidth="1"/>
+    <col min="7427" max="7427" width="20.54296875" customWidth="1"/>
     <col min="7428" max="7428" width="17" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7431" max="7431" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="21.42578125" customWidth="1"/>
-    <col min="7682" max="7682" width="14.85546875" customWidth="1"/>
-    <col min="7683" max="7683" width="20.5703125" customWidth="1"/>
+    <col min="7429" max="7429" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="21.453125" customWidth="1"/>
+    <col min="7682" max="7682" width="14.81640625" customWidth="1"/>
+    <col min="7683" max="7683" width="20.54296875" customWidth="1"/>
     <col min="7684" max="7684" width="17" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7687" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="21.42578125" customWidth="1"/>
-    <col min="7938" max="7938" width="14.85546875" customWidth="1"/>
-    <col min="7939" max="7939" width="20.5703125" customWidth="1"/>
+    <col min="7685" max="7685" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="21.453125" customWidth="1"/>
+    <col min="7938" max="7938" width="14.81640625" customWidth="1"/>
+    <col min="7939" max="7939" width="20.54296875" customWidth="1"/>
     <col min="7940" max="7940" width="17" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7943" max="7943" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="21.42578125" customWidth="1"/>
-    <col min="8194" max="8194" width="14.85546875" customWidth="1"/>
-    <col min="8195" max="8195" width="20.5703125" customWidth="1"/>
+    <col min="7941" max="7941" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="21.453125" customWidth="1"/>
+    <col min="8194" max="8194" width="14.81640625" customWidth="1"/>
+    <col min="8195" max="8195" width="20.54296875" customWidth="1"/>
     <col min="8196" max="8196" width="17" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8199" max="8199" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="21.42578125" customWidth="1"/>
-    <col min="8450" max="8450" width="14.85546875" customWidth="1"/>
-    <col min="8451" max="8451" width="20.5703125" customWidth="1"/>
+    <col min="8197" max="8197" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="21.453125" customWidth="1"/>
+    <col min="8450" max="8450" width="14.81640625" customWidth="1"/>
+    <col min="8451" max="8451" width="20.54296875" customWidth="1"/>
     <col min="8452" max="8452" width="17" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8455" max="8455" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="21.42578125" customWidth="1"/>
-    <col min="8706" max="8706" width="14.85546875" customWidth="1"/>
-    <col min="8707" max="8707" width="20.5703125" customWidth="1"/>
+    <col min="8453" max="8453" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="21.453125" customWidth="1"/>
+    <col min="8706" max="8706" width="14.81640625" customWidth="1"/>
+    <col min="8707" max="8707" width="20.54296875" customWidth="1"/>
     <col min="8708" max="8708" width="17" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8711" max="8711" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="21.42578125" customWidth="1"/>
-    <col min="8962" max="8962" width="14.85546875" customWidth="1"/>
-    <col min="8963" max="8963" width="20.5703125" customWidth="1"/>
+    <col min="8709" max="8709" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="21.453125" customWidth="1"/>
+    <col min="8962" max="8962" width="14.81640625" customWidth="1"/>
+    <col min="8963" max="8963" width="20.54296875" customWidth="1"/>
     <col min="8964" max="8964" width="17" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8967" max="8967" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="21.42578125" customWidth="1"/>
-    <col min="9218" max="9218" width="14.85546875" customWidth="1"/>
-    <col min="9219" max="9219" width="20.5703125" customWidth="1"/>
+    <col min="8965" max="8965" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="21.453125" customWidth="1"/>
+    <col min="9218" max="9218" width="14.81640625" customWidth="1"/>
+    <col min="9219" max="9219" width="20.54296875" customWidth="1"/>
     <col min="9220" max="9220" width="17" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9223" max="9223" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="21.42578125" customWidth="1"/>
-    <col min="9474" max="9474" width="14.85546875" customWidth="1"/>
-    <col min="9475" max="9475" width="20.5703125" customWidth="1"/>
+    <col min="9221" max="9221" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="21.453125" customWidth="1"/>
+    <col min="9474" max="9474" width="14.81640625" customWidth="1"/>
+    <col min="9475" max="9475" width="20.54296875" customWidth="1"/>
     <col min="9476" max="9476" width="17" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9479" max="9479" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="21.42578125" customWidth="1"/>
-    <col min="9730" max="9730" width="14.85546875" customWidth="1"/>
-    <col min="9731" max="9731" width="20.5703125" customWidth="1"/>
+    <col min="9477" max="9477" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="21.453125" customWidth="1"/>
+    <col min="9730" max="9730" width="14.81640625" customWidth="1"/>
+    <col min="9731" max="9731" width="20.54296875" customWidth="1"/>
     <col min="9732" max="9732" width="17" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9735" max="9735" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="21.42578125" customWidth="1"/>
-    <col min="9986" max="9986" width="14.85546875" customWidth="1"/>
-    <col min="9987" max="9987" width="20.5703125" customWidth="1"/>
+    <col min="9733" max="9733" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="21.453125" customWidth="1"/>
+    <col min="9986" max="9986" width="14.81640625" customWidth="1"/>
+    <col min="9987" max="9987" width="20.54296875" customWidth="1"/>
     <col min="9988" max="9988" width="17" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9991" max="9991" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="21.42578125" customWidth="1"/>
-    <col min="10242" max="10242" width="14.85546875" customWidth="1"/>
-    <col min="10243" max="10243" width="20.5703125" customWidth="1"/>
+    <col min="9989" max="9989" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="21.453125" customWidth="1"/>
+    <col min="10242" max="10242" width="14.81640625" customWidth="1"/>
+    <col min="10243" max="10243" width="20.54296875" customWidth="1"/>
     <col min="10244" max="10244" width="17" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10247" max="10247" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="21.42578125" customWidth="1"/>
-    <col min="10498" max="10498" width="14.85546875" customWidth="1"/>
-    <col min="10499" max="10499" width="20.5703125" customWidth="1"/>
+    <col min="10245" max="10245" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="21.453125" customWidth="1"/>
+    <col min="10498" max="10498" width="14.81640625" customWidth="1"/>
+    <col min="10499" max="10499" width="20.54296875" customWidth="1"/>
     <col min="10500" max="10500" width="17" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10503" max="10503" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="21.42578125" customWidth="1"/>
-    <col min="10754" max="10754" width="14.85546875" customWidth="1"/>
-    <col min="10755" max="10755" width="20.5703125" customWidth="1"/>
+    <col min="10501" max="10501" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="21.453125" customWidth="1"/>
+    <col min="10754" max="10754" width="14.81640625" customWidth="1"/>
+    <col min="10755" max="10755" width="20.54296875" customWidth="1"/>
     <col min="10756" max="10756" width="17" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10759" max="10759" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="21.42578125" customWidth="1"/>
-    <col min="11010" max="11010" width="14.85546875" customWidth="1"/>
-    <col min="11011" max="11011" width="20.5703125" customWidth="1"/>
+    <col min="10757" max="10757" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="21.453125" customWidth="1"/>
+    <col min="11010" max="11010" width="14.81640625" customWidth="1"/>
+    <col min="11011" max="11011" width="20.54296875" customWidth="1"/>
     <col min="11012" max="11012" width="17" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11015" max="11015" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="21.42578125" customWidth="1"/>
-    <col min="11266" max="11266" width="14.85546875" customWidth="1"/>
-    <col min="11267" max="11267" width="20.5703125" customWidth="1"/>
+    <col min="11013" max="11013" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="21.453125" customWidth="1"/>
+    <col min="11266" max="11266" width="14.81640625" customWidth="1"/>
+    <col min="11267" max="11267" width="20.54296875" customWidth="1"/>
     <col min="11268" max="11268" width="17" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11271" max="11271" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="21.42578125" customWidth="1"/>
-    <col min="11522" max="11522" width="14.85546875" customWidth="1"/>
-    <col min="11523" max="11523" width="20.5703125" customWidth="1"/>
+    <col min="11269" max="11269" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="21.453125" customWidth="1"/>
+    <col min="11522" max="11522" width="14.81640625" customWidth="1"/>
+    <col min="11523" max="11523" width="20.54296875" customWidth="1"/>
     <col min="11524" max="11524" width="17" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11527" max="11527" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="21.42578125" customWidth="1"/>
-    <col min="11778" max="11778" width="14.85546875" customWidth="1"/>
-    <col min="11779" max="11779" width="20.5703125" customWidth="1"/>
+    <col min="11525" max="11525" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="21.453125" customWidth="1"/>
+    <col min="11778" max="11778" width="14.81640625" customWidth="1"/>
+    <col min="11779" max="11779" width="20.54296875" customWidth="1"/>
     <col min="11780" max="11780" width="17" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11783" max="11783" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="21.42578125" customWidth="1"/>
-    <col min="12034" max="12034" width="14.85546875" customWidth="1"/>
-    <col min="12035" max="12035" width="20.5703125" customWidth="1"/>
+    <col min="11781" max="11781" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="21.453125" customWidth="1"/>
+    <col min="12034" max="12034" width="14.81640625" customWidth="1"/>
+    <col min="12035" max="12035" width="20.54296875" customWidth="1"/>
     <col min="12036" max="12036" width="17" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12039" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="21.42578125" customWidth="1"/>
-    <col min="12290" max="12290" width="14.85546875" customWidth="1"/>
-    <col min="12291" max="12291" width="20.5703125" customWidth="1"/>
+    <col min="12037" max="12037" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="21.453125" customWidth="1"/>
+    <col min="12290" max="12290" width="14.81640625" customWidth="1"/>
+    <col min="12291" max="12291" width="20.54296875" customWidth="1"/>
     <col min="12292" max="12292" width="17" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12295" max="12295" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="21.42578125" customWidth="1"/>
-    <col min="12546" max="12546" width="14.85546875" customWidth="1"/>
-    <col min="12547" max="12547" width="20.5703125" customWidth="1"/>
+    <col min="12293" max="12293" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="21.453125" customWidth="1"/>
+    <col min="12546" max="12546" width="14.81640625" customWidth="1"/>
+    <col min="12547" max="12547" width="20.54296875" customWidth="1"/>
     <col min="12548" max="12548" width="17" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12551" max="12551" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="21.42578125" customWidth="1"/>
-    <col min="12802" max="12802" width="14.85546875" customWidth="1"/>
-    <col min="12803" max="12803" width="20.5703125" customWidth="1"/>
+    <col min="12549" max="12549" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="21.453125" customWidth="1"/>
+    <col min="12802" max="12802" width="14.81640625" customWidth="1"/>
+    <col min="12803" max="12803" width="20.54296875" customWidth="1"/>
     <col min="12804" max="12804" width="17" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12807" max="12807" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="21.42578125" customWidth="1"/>
-    <col min="13058" max="13058" width="14.85546875" customWidth="1"/>
-    <col min="13059" max="13059" width="20.5703125" customWidth="1"/>
+    <col min="12805" max="12805" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="21.453125" customWidth="1"/>
+    <col min="13058" max="13058" width="14.81640625" customWidth="1"/>
+    <col min="13059" max="13059" width="20.54296875" customWidth="1"/>
     <col min="13060" max="13060" width="17" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13063" max="13063" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="21.42578125" customWidth="1"/>
-    <col min="13314" max="13314" width="14.85546875" customWidth="1"/>
-    <col min="13315" max="13315" width="20.5703125" customWidth="1"/>
+    <col min="13061" max="13061" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="21.453125" customWidth="1"/>
+    <col min="13314" max="13314" width="14.81640625" customWidth="1"/>
+    <col min="13315" max="13315" width="20.54296875" customWidth="1"/>
     <col min="13316" max="13316" width="17" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13319" max="13319" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="21.42578125" customWidth="1"/>
-    <col min="13570" max="13570" width="14.85546875" customWidth="1"/>
-    <col min="13571" max="13571" width="20.5703125" customWidth="1"/>
+    <col min="13317" max="13317" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="21.453125" customWidth="1"/>
+    <col min="13570" max="13570" width="14.81640625" customWidth="1"/>
+    <col min="13571" max="13571" width="20.54296875" customWidth="1"/>
     <col min="13572" max="13572" width="17" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13575" max="13575" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="21.42578125" customWidth="1"/>
-    <col min="13826" max="13826" width="14.85546875" customWidth="1"/>
-    <col min="13827" max="13827" width="20.5703125" customWidth="1"/>
+    <col min="13573" max="13573" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="21.453125" customWidth="1"/>
+    <col min="13826" max="13826" width="14.81640625" customWidth="1"/>
+    <col min="13827" max="13827" width="20.54296875" customWidth="1"/>
     <col min="13828" max="13828" width="17" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13831" max="13831" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="21.42578125" customWidth="1"/>
-    <col min="14082" max="14082" width="14.85546875" customWidth="1"/>
-    <col min="14083" max="14083" width="20.5703125" customWidth="1"/>
+    <col min="13829" max="13829" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="21.453125" customWidth="1"/>
+    <col min="14082" max="14082" width="14.81640625" customWidth="1"/>
+    <col min="14083" max="14083" width="20.54296875" customWidth="1"/>
     <col min="14084" max="14084" width="17" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14087" max="14087" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="21.42578125" customWidth="1"/>
-    <col min="14338" max="14338" width="14.85546875" customWidth="1"/>
-    <col min="14339" max="14339" width="20.5703125" customWidth="1"/>
+    <col min="14085" max="14085" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="21.453125" customWidth="1"/>
+    <col min="14338" max="14338" width="14.81640625" customWidth="1"/>
+    <col min="14339" max="14339" width="20.54296875" customWidth="1"/>
     <col min="14340" max="14340" width="17" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14343" max="14343" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="21.42578125" customWidth="1"/>
-    <col min="14594" max="14594" width="14.85546875" customWidth="1"/>
-    <col min="14595" max="14595" width="20.5703125" customWidth="1"/>
+    <col min="14341" max="14341" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="21.453125" customWidth="1"/>
+    <col min="14594" max="14594" width="14.81640625" customWidth="1"/>
+    <col min="14595" max="14595" width="20.54296875" customWidth="1"/>
     <col min="14596" max="14596" width="17" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14599" max="14599" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="21.42578125" customWidth="1"/>
-    <col min="14850" max="14850" width="14.85546875" customWidth="1"/>
-    <col min="14851" max="14851" width="20.5703125" customWidth="1"/>
+    <col min="14597" max="14597" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="21.453125" customWidth="1"/>
+    <col min="14850" max="14850" width="14.81640625" customWidth="1"/>
+    <col min="14851" max="14851" width="20.54296875" customWidth="1"/>
     <col min="14852" max="14852" width="17" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14855" max="14855" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="21.42578125" customWidth="1"/>
-    <col min="15106" max="15106" width="14.85546875" customWidth="1"/>
-    <col min="15107" max="15107" width="20.5703125" customWidth="1"/>
+    <col min="14853" max="14853" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="21.453125" customWidth="1"/>
+    <col min="15106" max="15106" width="14.81640625" customWidth="1"/>
+    <col min="15107" max="15107" width="20.54296875" customWidth="1"/>
     <col min="15108" max="15108" width="17" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15111" max="15111" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="21.42578125" customWidth="1"/>
-    <col min="15362" max="15362" width="14.85546875" customWidth="1"/>
-    <col min="15363" max="15363" width="20.5703125" customWidth="1"/>
+    <col min="15109" max="15109" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="21.453125" customWidth="1"/>
+    <col min="15362" max="15362" width="14.81640625" customWidth="1"/>
+    <col min="15363" max="15363" width="20.54296875" customWidth="1"/>
     <col min="15364" max="15364" width="17" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15367" max="15367" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="21.42578125" customWidth="1"/>
-    <col min="15618" max="15618" width="14.85546875" customWidth="1"/>
-    <col min="15619" max="15619" width="20.5703125" customWidth="1"/>
+    <col min="15365" max="15365" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="21.453125" customWidth="1"/>
+    <col min="15618" max="15618" width="14.81640625" customWidth="1"/>
+    <col min="15619" max="15619" width="20.54296875" customWidth="1"/>
     <col min="15620" max="15620" width="17" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15623" max="15623" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="21.42578125" customWidth="1"/>
-    <col min="15874" max="15874" width="14.85546875" customWidth="1"/>
-    <col min="15875" max="15875" width="20.5703125" customWidth="1"/>
+    <col min="15621" max="15621" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="21.453125" customWidth="1"/>
+    <col min="15874" max="15874" width="14.81640625" customWidth="1"/>
+    <col min="15875" max="15875" width="20.54296875" customWidth="1"/>
     <col min="15876" max="15876" width="17" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15879" max="15879" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="21.42578125" customWidth="1"/>
-    <col min="16130" max="16130" width="14.85546875" customWidth="1"/>
-    <col min="16131" max="16131" width="20.5703125" customWidth="1"/>
+    <col min="15877" max="15877" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="21.453125" customWidth="1"/>
+    <col min="16130" max="16130" width="14.81640625" customWidth="1"/>
+    <col min="16131" max="16131" width="20.54296875" customWidth="1"/>
     <col min="16132" max="16132" width="17" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16135" max="16135" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -12947,7 +12985,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>887</v>
       </c>
@@ -12976,7 +13014,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1086</v>
       </c>
@@ -13005,7 +13043,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1086</v>
       </c>
@@ -13034,7 +13072,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1086</v>
       </c>
@@ -13063,7 +13101,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>887</v>
       </c>
@@ -13092,7 +13130,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>887</v>
       </c>
@@ -13121,7 +13159,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>887</v>
       </c>
@@ -13150,7 +13188,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>893</v>
       </c>
@@ -13179,7 +13217,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>910</v>
       </c>
@@ -13208,7 +13246,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>910</v>
       </c>
@@ -13237,7 +13275,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>893</v>
       </c>
@@ -13289,22 +13327,22 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13354,7 +13392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>562</v>
       </c>
@@ -13389,7 +13427,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>572</v>
       </c>
@@ -13424,7 +13462,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>659</v>
       </c>
@@ -13459,7 +13497,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>995</v>
       </c>
@@ -13494,7 +13532,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>740</v>
       </c>
@@ -13529,7 +13567,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>835</v>
       </c>
@@ -13562,7 +13600,7 @@
       </c>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>879</v>
       </c>
@@ -13597,7 +13635,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1028</v>
       </c>
@@ -13632,7 +13670,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>1040</v>
       </c>
@@ -13664,7 +13702,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1053</v>
       </c>
@@ -13699,7 +13737,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1182</v>
       </c>
@@ -13734,7 +13772,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1190</v>
       </c>
@@ -13769,7 +13807,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1196</v>
       </c>
@@ -13818,9 +13856,9 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13889,22 +13927,22 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13957,7 +13995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -13995,7 +14033,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -14033,7 +14071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -14071,7 +14109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>610</v>
       </c>
@@ -14109,7 +14147,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>717</v>
       </c>
@@ -14147,7 +14185,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>731</v>
       </c>
@@ -14185,7 +14223,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>746</v>
       </c>
@@ -14223,7 +14261,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>751</v>
       </c>
@@ -14261,7 +14299,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>755</v>
       </c>
@@ -14299,7 +14337,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>877</v>
       </c>
@@ -14337,7 +14375,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>885</v>
       </c>
@@ -14375,7 +14413,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>931</v>
       </c>
@@ -14413,7 +14451,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>973</v>
       </c>
@@ -14451,7 +14489,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>990</v>
       </c>
@@ -14486,7 +14524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1019</v>
       </c>
@@ -14524,7 +14562,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1072</v>
       </c>
@@ -14562,7 +14600,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1109</v>
       </c>
@@ -14600,7 +14638,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1117</v>
       </c>
@@ -14638,7 +14676,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1120</v>
       </c>
@@ -14676,7 +14714,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1123</v>
       </c>
@@ -14714,7 +14752,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1126</v>
       </c>
@@ -14752,7 +14790,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1146</v>
       </c>
@@ -14804,22 +14842,22 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14872,7 +14910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>744272121</v>
       </c>
@@ -14907,7 +14945,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>635</v>
       </c>
@@ -14945,7 +14983,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>701</v>
       </c>
@@ -14980,7 +15018,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>759</v>
       </c>
@@ -15018,7 +15056,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1043</v>
       </c>
@@ -15056,7 +15094,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1177</v>
       </c>
@@ -15094,7 +15132,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1209</v>
       </c>
@@ -15129,7 +15167,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="28" ht="13.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="13.4" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15144,9 +15182,9 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15166,7 +15204,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>764</v>
       </c>
@@ -15199,18 +15237,18 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -15239,7 +15277,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>589</v>
       </c>
@@ -15268,7 +15306,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>589</v>
       </c>
@@ -15297,7 +15335,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>841</v>
       </c>
@@ -15326,7 +15364,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1201</v>
       </c>
@@ -15352,7 +15390,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1201</v>
       </c>
@@ -15394,21 +15432,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -15443,7 +15481,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>794</v>
       </c>
@@ -15478,7 +15516,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>790</v>
       </c>
@@ -15513,7 +15551,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>928</v>
       </c>
@@ -15565,21 +15603,21 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15626,7 +15664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>581</v>
       </c>
@@ -15658,7 +15696,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>603</v>
       </c>
@@ -15687,7 +15725,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>708</v>
       </c>
@@ -15719,7 +15757,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>828</v>
       </c>
@@ -15749,7 +15787,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>857</v>
       </c>
@@ -15778,7 +15816,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1007</v>
       </c>
@@ -15807,7 +15845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1012</v>
       </c>
@@ -15836,7 +15874,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1016</v>
       </c>
@@ -15859,7 +15897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1082</v>
       </c>
@@ -15899,14 +15937,14 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15947,7 +15985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>648</v>
       </c>
@@ -15978,7 +16016,7 @@
       <c r="U2" s="7"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>649</v>
       </c>
@@ -16009,7 +16047,7 @@
       <c r="U3" s="7"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>650</v>
       </c>
@@ -16040,7 +16078,7 @@
       <c r="U4" s="7"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>651</v>
       </c>
@@ -16071,7 +16109,7 @@
       <c r="U5" s="7"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>652</v>
       </c>
@@ -16102,11 +16140,11 @@
       <c r="U6" s="7"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="E7" s="7"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="E8" s="7"/>
       <c r="H8" s="5"/>
     </row>
@@ -16123,22 +16161,22 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16185,7 +16223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>595</v>
       </c>
@@ -16217,7 +16255,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>666</v>
       </c>
@@ -16249,7 +16287,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>863</v>
       </c>
@@ -16281,7 +16319,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>958</v>
       </c>
@@ -16313,7 +16351,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1140</v>
       </c>
@@ -16345,7 +16383,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="I9" s="5"/>
     </row>
   </sheetData>

</xml_diff>